<commit_message>
Added altitude relative test data
</commit_message>
<xml_diff>
--- a/Testing/Relative Positioning/Altitude Relative Measure/Altitude Relative Measure Calculations.xlsx
+++ b/Testing/Relative Positioning/Altitude Relative Measure/Altitude Relative Measure Calculations.xlsx
@@ -4,21 +4,22 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="630" yWindow="600" windowWidth="27495" windowHeight="13740" activeTab="4"/>
+    <workbookView xWindow="630" yWindow="600" windowWidth="27495" windowHeight="13740" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Az=0 (4-3-18)" sheetId="1" r:id="rId1"/>
-    <sheet name="Az=0 (4-4-18 retest)" sheetId="2" r:id="rId2"/>
-    <sheet name="Az=10 (4-4-18)" sheetId="3" r:id="rId3"/>
-    <sheet name="Az=10 (4-6-18)(angle apparatus)" sheetId="4" r:id="rId4"/>
-    <sheet name="Grid Measurements" sheetId="5" r:id="rId5"/>
+    <sheet name="Az=0 Plot with Error bars" sheetId="6" r:id="rId2"/>
+    <sheet name="Az=0 (4-4-18 retest)" sheetId="2" r:id="rId3"/>
+    <sheet name="Az=10 (4-4-18)" sheetId="3" r:id="rId4"/>
+    <sheet name="Az=10 (4-6-18)(angle apparatus)" sheetId="4" r:id="rId5"/>
+    <sheet name="Grid Measurements" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="35">
   <si>
     <t>TAN</t>
   </si>
@@ -106,12 +107,50 @@
   <si>
     <t>Numbers are width of horizontal movement when commanded to each position.</t>
   </si>
+  <si>
+    <t xml:space="preserve">Command Angle [deg] </t>
+  </si>
+  <si>
+    <t>Theoretical Height Above Zero [mm]</t>
+  </si>
+  <si>
+    <t>Measured Height Above Ref [mm]</t>
+  </si>
+  <si>
+    <t>Height from Zero to Ref [mm]</t>
+  </si>
+  <si>
+    <t>% Error</t>
+  </si>
+  <si>
+    <r>
+      <t>Altitude Relative Position Test, Azimuth = 0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>°</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>, DistanceToBoard = 1295mm</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -120,6 +159,23 @@
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -130,7 +186,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -138,21 +194,163 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -251,11 +449,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="162206080"/>
-        <c:axId val="162208000"/>
+        <c:axId val="145450880"/>
+        <c:axId val="145453056"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="162206080"/>
+        <c:axId val="145450880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -289,12 +487,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="162208000"/>
+        <c:crossAx val="145453056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="162208000"/>
+        <c:axId val="145453056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -328,7 +526,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="162206080"/>
+        <c:crossAx val="145450880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -359,8 +557,15 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
-  <c:roundedCorners val="1"/>
-  <c:style val="2"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:autoTitleDeleted val="1"/>
     <c:plotArea>
@@ -369,133 +574,192 @@
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="0"/>
+          <c:idx val="1"/>
           <c:order val="0"/>
           <c:spPr>
-            <a:ln w="47625">
+            <a:ln w="28575">
               <a:noFill/>
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="7"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="4F81BD"/>
-              </a:solidFill>
-              <a:ln cmpd="sng">
-                <a:solidFill>
-                  <a:srgbClr val="4F81BD"/>
-                </a:solidFill>
-              </a:ln>
-            </c:spPr>
+            <c:symbol val="dash"/>
+            <c:size val="5"/>
           </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-              </a:ln>
-            </c:spPr>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="1"/>
-            <c:dispEq val="0"/>
-            <c:trendlineLbl>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-            </c:trendlineLbl>
-          </c:trendline>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>'Az=10 (4-4-18)'!$C$14:$C$24</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="11"/>
+                  <c:pt idx="0">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>-0.41630063829126129</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>1.6525434578410909</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>2.155105334736561</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>4.5049834595457128</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>6.1736362104368823</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>8.7040792421740321</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>8.7281760628829943</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>13.988739797602193</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>17.368148019697855</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>21.982069618405149</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>'Az=10 (4-4-18)'!$C$14:$C$24</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="11"/>
+                  <c:pt idx="0">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>-0.41630063829126129</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>1.6525434578410909</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>2.155105334736561</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>4.5049834595457128</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>6.1736362104368823</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>8.7040792421740321</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>8.7281760628829943</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>13.988739797602193</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>17.368148019697855</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>21.982069618405149</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+          </c:errBars>
           <c:xVal>
             <c:numRef>
-              <c:f>'Az=0 (4-4-18 retest)'!$D$2:$D$13</c:f>
+              <c:f>'Az=10 (4-4-18)'!$B$2:$B$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>395.92123248896519</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>471.34145337473205</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>536.4065632731581</c:v>
+                  <c:v>22.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>603.8684173107232</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>674.13433046451132</c:v>
+                  <c:v>27.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>747.66859860056536</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>825.00598774570369</c:v>
+                  <c:v>32.5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>906.76876198157413</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>993.68844943275371</c:v>
+                  <c:v>37.5</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1086.6340223745774</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1166.0232373657027</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1294.9999999999998</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Az=0 (4-4-18 retest)'!$G$2:$G$13</c:f>
+              <c:f>'Az=10 (4-4-18)'!$B$14:$B$24</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.99853562005101781</c:v>
+                  <c:v>76.583699361708739</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.0012258266149099</c:v>
+                  <c:v>142.65254345784109</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.0074438665570686</c:v>
+                  <c:v>211.15510533473656</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.0055897430951946</c:v>
+                  <c:v>282.50498345954571</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.0044134185494811</c:v>
+                  <c:v>357.17363621043688</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.0153686005130025</c:v>
+                  <c:v>435.70407924217403</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.0172951812903841</c:v>
+                  <c:v>518.72817606288299</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.0297211060639859</c:v>
+                  <c:v>606.98873979760219</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.0371609014073835</c:v>
+                  <c:v>701.36814801969786</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.0532984925917699</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1.065868575289812</c:v>
+                  <c:v>781.98206961840515</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="1"/>
+          <c:smooth val="0"/>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -505,106 +769,88 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="162229248"/>
-        <c:axId val="162407168"/>
+        <c:axId val="135836032"/>
+        <c:axId val="135837568"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="162229248"/>
+        <c:axId val="135836032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Commanded Angle [deg]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="cross"/>
-        <c:minorTickMark val="cross"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="47625">
-            <a:noFill/>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr lvl="0">
-              <a:defRPr b="0"/>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="162407168"/>
+        <c:crossAx val="135837568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="162407168"/>
+        <c:axId val="135837568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:srgbClr val="B7B7B7"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="cross"/>
-        <c:minorTickMark val="cross"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Expected</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Distance Above Reference Point [mm]</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="47625">
-            <a:noFill/>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr lvl="0">
-              <a:defRPr b="0"/>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="162229248"/>
+        <c:crossAx val="135836032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
-      <c:spPr>
-        <a:solidFill>
-          <a:srgbClr val="FFFFFF"/>
-        </a:solidFill>
-      </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-    </c:legend>
     <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="zero"/>
-    <c:showDLblsOverMax val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
 </c:chartSpace>
 </file>
 
@@ -643,101 +889,92 @@
               </a:ln>
             </c:spPr>
           </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-              </a:ln>
-            </c:spPr>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="1"/>
-            <c:dispEq val="0"/>
-            <c:trendlineLbl>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-            </c:trendlineLbl>
-          </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Az=10 (4-4-18)'!$D$2:$D$12</c:f>
+              <c:f>'Az=0 (4-4-18 retest)'!$D$3:$D$14</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>402.02895567989827</c:v>
+                  <c:v>395.92123248896519</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>478.61265504160701</c:v>
+                  <c:v>471.34145337473205</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>544.68149913773937</c:v>
+                  <c:v>536.4065632731581</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>613.18406101463484</c:v>
+                  <c:v>603.8684173107232</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>684.53393913944399</c:v>
+                  <c:v>674.13433046451132</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>759.20259189033516</c:v>
+                  <c:v>747.66859860056536</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>837.73303492207231</c:v>
+                  <c:v>825.00598774570369</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>920.75713174278133</c:v>
+                  <c:v>906.76876198157413</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1009.0176954775005</c:v>
+                  <c:v>993.68844943275371</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1103.3971036995961</c:v>
+                  <c:v>1086.6340223745774</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1184.0110252983034</c:v>
+                  <c:v>1166.0232373657027</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1294.9999999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Az=10 (4-4-18)'!$G$2:$G$12</c:f>
+              <c:f>'Az=0 (4-4-18 retest)'!$G$3:$G$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.9989645008589314</c:v>
+                  <c:v>-0.14643799489821313</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.0041105085454514</c:v>
+                  <c:v>0.12258266149099181</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.0053605724271575</c:v>
+                  <c:v>0.74438665570686613</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.0112056193861136</c:v>
+                  <c:v>0.55897430951946125</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.0153561979136458</c:v>
+                  <c:v>0.44134185494809841</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.021650378957043</c:v>
+                  <c:v>1.5368600513002528</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.0217103169798361</c:v>
+                  <c:v>1.7295181290384043</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.0347953539165977</c:v>
+                  <c:v>2.9721106063985827</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.0432012365634842</c:v>
+                  <c:v>3.7160901407383533</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.0546778268277461</c:v>
+                  <c:v>5.3298492591769877</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6.5868575289812048</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -752,11 +989,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="162424320"/>
-        <c:axId val="162425856"/>
+        <c:axId val="145969920"/>
+        <c:axId val="145971456"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="162424320"/>
+        <c:axId val="145969920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -771,7 +1008,7 @@
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="cross"/>
         <c:minorTickMark val="cross"/>
         <c:tickLblPos val="nextTo"/>
@@ -790,12 +1027,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="162425856"/>
+        <c:crossAx val="145971456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="162425856"/>
+        <c:axId val="145971456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -829,7 +1066,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="162424320"/>
+        <c:crossAx val="145969920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -841,6 +1078,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -902,14 +1140,15 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="0"/>
             <c:trendlineLbl>
+              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Az=10 (4-6-18)(angle apparatus)'!$D$2:$D$12</c:f>
+              <c:f>'Az=10 (4-4-18)'!$D$2:$D$12</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>402.02895567989827</c:v>
@@ -949,42 +1188,42 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Az=10 (4-6-18)(angle apparatus)'!$G$2:$G$12</c:f>
+              <c:f>'Az=10 (4-4-18)'!$G$2:$G$12</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.9989645008589314</c:v>
+                  <c:v>-1.0354991410686507E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.0041105085454514</c:v>
+                  <c:v>4.1105085454513175E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.0053605724271575</c:v>
+                  <c:v>5.3605724271574345E-3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.0112056193861136</c:v>
+                  <c:v>1.1205619386113698E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.0153561979136458</c:v>
+                  <c:v>1.5356197913645871E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.021650378957043</c:v>
+                  <c:v>2.1650378957042974E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.0217103169798361</c:v>
+                  <c:v>2.1710316979836053E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.0347953539165977</c:v>
+                  <c:v>3.4795353916597743E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.0432012365634842</c:v>
+                  <c:v>4.3201236563484222E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.0546778268277461</c:v>
+                  <c:v>5.4677826827746107E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -999,11 +1238,260 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="162579968"/>
-        <c:axId val="162581504"/>
+        <c:axId val="146017280"/>
+        <c:axId val="146019072"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="162579968"/>
+        <c:axId val="146017280"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="cross"/>
+        <c:minorTickMark val="cross"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="47625">
+            <a:noFill/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="146019072"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="146019072"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="B7B7B7"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+        <c:majorTickMark val="cross"/>
+        <c:minorTickMark val="cross"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="47625">
+            <a:noFill/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="146017280"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="1"/>
+  <c:style val="2"/>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="47625">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="7"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="4F81BD"/>
+              </a:solidFill>
+              <a:ln cmpd="sng">
+                <a:solidFill>
+                  <a:srgbClr val="4F81BD"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="0"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Az=10 (4-6-18)(angle apparatus)'!$D$2:$D$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>402.02895567989827</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>478.61265504160701</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>544.68149913773937</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>613.18406101463484</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>684.53393913944399</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>759.20259189033516</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>837.73303492207231</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>920.75713174278133</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1009.0176954775005</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1103.3971036995961</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1184.0110252983034</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Az=10 (4-6-18)(angle apparatus)'!$G$2:$G$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.9989645008589314</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0041105085454514</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0053605724271575</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.0112056193861136</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.0153561979136458</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.021650378957043</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.0217103169798361</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.0347953539165977</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.0432012365634842</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.0546778268277461</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="146086912"/>
+        <c:axId val="146092800"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="146086912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1037,12 +1525,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="162581504"/>
+        <c:crossAx val="146092800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="162581504"/>
+        <c:axId val="146092800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1076,7 +1564,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="162579968"/>
+        <c:crossAx val="146086912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1088,6 +1576,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1100,6 +1589,17 @@
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
+</file>
+
+<file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="145" workbookViewId="0"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1134,12 +1634,39 @@
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8671560" cy="6294120"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>590550</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="4343400" cy="2886075"/>
     <xdr:graphicFrame macro="">
@@ -1162,7 +1689,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
@@ -1192,7 +1719,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
@@ -1511,7 +2038,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -2654,507 +3183,619 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K1000"/>
+  <dimension ref="A1:T1001"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T3" sqref="T3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="2" max="3" width="8.7109375" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" customWidth="1"/>
-    <col min="5" max="5" width="21.85546875" customWidth="1"/>
-    <col min="6" max="6" width="19" customWidth="1"/>
+    <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="34" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
-      <c r="C1" t="s">
+    <row r="1" spans="1:20" s="3" customFormat="1" ht="15" customHeight="1">
+      <c r="B1" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="10"/>
+    </row>
+    <row r="2" spans="1:20">
+      <c r="B2" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" t="s">
-        <v>4</v>
-      </c>
-      <c r="K1" t="s">
+      <c r="D2" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="K2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:11">
-      <c r="A2">
-        <f t="shared" ref="A2:A13" si="0">RADIANS(B2)</f>
+      <c r="S2" s="17">
+        <f>D3-$D$3</f>
+        <v>0</v>
+      </c>
+      <c r="T2" s="17">
+        <f>S2-E3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20">
+      <c r="A3">
+        <f t="shared" ref="A3:A14" si="0">RADIANS(B3)</f>
         <v>0.29670597283903605</v>
       </c>
-      <c r="B2">
+      <c r="B3" s="11">
         <v>17</v>
       </c>
-      <c r="C2">
-        <f t="shared" ref="C2:C13" si="1">TAN(RADIANS(B2))</f>
+      <c r="C3" s="7">
+        <f t="shared" ref="C3:C14" si="1">TAN(RADIANS(B3))</f>
         <v>0.30573068145866039</v>
       </c>
-      <c r="D2">
-        <f t="shared" ref="D2:D13" si="2">C2*$K$2</f>
+      <c r="D3" s="15">
+        <f t="shared" ref="D3:D14" si="2">C3*$K$3</f>
         <v>395.92123248896519</v>
       </c>
-      <c r="E2">
+      <c r="E3" s="7">
         <v>0</v>
       </c>
-      <c r="F2">
-        <f t="shared" ref="F2:F13" si="3">D2-E2</f>
+      <c r="F3" s="15">
+        <f t="shared" ref="F3:F14" si="3">D3-E3</f>
         <v>395.92123248896519</v>
       </c>
-      <c r="G2">
-        <f t="shared" ref="G2:G13" si="4">F2/$D$2</f>
-        <v>1</v>
-      </c>
-      <c r="K2">
+      <c r="G3" s="18">
+        <f>(F3-$D$3)/$D$3*100</f>
+        <v>0</v>
+      </c>
+      <c r="K3">
         <v>1295</v>
       </c>
-    </row>
-    <row r="3" spans="1:11">
-      <c r="A3">
+      <c r="S3" s="17">
+        <f t="shared" ref="S3:S14" si="4">D4-$D$3</f>
+        <v>75.420220885766867</v>
+      </c>
+      <c r="T3" s="17">
+        <f>S3-E4</f>
+        <v>-0.57977911423313344</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20">
+      <c r="A4">
         <f t="shared" si="0"/>
         <v>0.3490658503988659</v>
       </c>
-      <c r="B3">
+      <c r="B4" s="11">
         <v>20</v>
       </c>
-      <c r="C3">
+      <c r="C4" s="7">
         <f t="shared" si="1"/>
         <v>0.36397023426620234</v>
       </c>
-      <c r="D3">
+      <c r="D4" s="15">
         <f t="shared" si="2"/>
         <v>471.34145337473205</v>
       </c>
-      <c r="E3">
+      <c r="E4" s="7">
         <v>76</v>
       </c>
-      <c r="F3">
+      <c r="F4" s="15">
         <f t="shared" si="3"/>
         <v>395.34145337473205</v>
       </c>
-      <c r="G3">
+      <c r="G4" s="18">
+        <f t="shared" ref="G4:G14" si="5">(F4-$D$3)/$D$3*100</f>
+        <v>-0.14643799489821313</v>
+      </c>
+      <c r="S4" s="17">
         <f t="shared" si="4"/>
-        <v>0.99853562005101781</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
-      <c r="A4">
+        <v>140.48533078419291</v>
+      </c>
+      <c r="T4" s="17">
+        <f t="shared" ref="T3:T13" si="6">S4-E5</f>
+        <v>0.48533078419291087</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20">
+      <c r="A5">
         <f t="shared" si="0"/>
         <v>0.39269908169872414</v>
       </c>
-      <c r="B4">
+      <c r="B5" s="11">
         <v>22.5</v>
       </c>
-      <c r="C4">
+      <c r="C5" s="7">
         <f t="shared" si="1"/>
         <v>0.41421356237309503</v>
       </c>
-      <c r="D4">
+      <c r="D5" s="15">
         <f t="shared" si="2"/>
         <v>536.4065632731581</v>
       </c>
-      <c r="E4">
+      <c r="E5" s="7">
         <v>140</v>
       </c>
-      <c r="F4">
+      <c r="F5" s="15">
         <f t="shared" si="3"/>
         <v>396.4065632731581</v>
       </c>
-      <c r="G4">
+      <c r="G5" s="18">
+        <f t="shared" si="5"/>
+        <v>0.12258266149099181</v>
+      </c>
+      <c r="S5" s="17">
         <f t="shared" si="4"/>
-        <v>1.0012258266149099</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
-      <c r="A5">
+        <v>207.94718482175801</v>
+      </c>
+      <c r="T5" s="17">
+        <f t="shared" si="6"/>
+        <v>2.9471848217580146</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20">
+      <c r="A6">
         <f t="shared" si="0"/>
         <v>0.43633231299858238</v>
       </c>
-      <c r="B5">
+      <c r="B6" s="11">
         <v>25</v>
       </c>
-      <c r="C5">
+      <c r="C6" s="7">
         <f t="shared" si="1"/>
         <v>0.46630765815499858</v>
       </c>
-      <c r="D5">
+      <c r="D6" s="15">
         <f t="shared" si="2"/>
         <v>603.8684173107232</v>
       </c>
-      <c r="E5">
+      <c r="E6" s="7">
         <v>205</v>
       </c>
-      <c r="F5">
+      <c r="F6" s="15">
         <f t="shared" si="3"/>
         <v>398.8684173107232</v>
       </c>
-      <c r="G5">
+      <c r="G6" s="18">
+        <f t="shared" si="5"/>
+        <v>0.74438665570686613</v>
+      </c>
+      <c r="S6" s="17">
         <f t="shared" si="4"/>
-        <v>1.0074438665570686</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11">
-      <c r="A6">
+        <v>278.21309797554613</v>
+      </c>
+      <c r="T6" s="17">
+        <f t="shared" si="6"/>
+        <v>2.213097975546134</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20">
+      <c r="A7">
         <f t="shared" si="0"/>
         <v>0.47996554429844063</v>
       </c>
-      <c r="B6">
+      <c r="B7" s="11">
         <v>27.5</v>
       </c>
-      <c r="C6">
+      <c r="C7" s="7">
         <f t="shared" si="1"/>
         <v>0.52056705055174624</v>
       </c>
-      <c r="D6">
+      <c r="D7" s="15">
         <f t="shared" si="2"/>
         <v>674.13433046451132</v>
       </c>
-      <c r="E6">
+      <c r="E7" s="7">
         <v>276</v>
       </c>
-      <c r="F6">
+      <c r="F7" s="15">
         <f t="shared" si="3"/>
         <v>398.13433046451132</v>
       </c>
-      <c r="G6">
+      <c r="G7" s="18">
+        <f t="shared" si="5"/>
+        <v>0.55897430951946125</v>
+      </c>
+      <c r="S7" s="17">
         <f t="shared" si="4"/>
-        <v>1.0055897430951946</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11">
-      <c r="A7">
+        <v>351.74736611160017</v>
+      </c>
+      <c r="T7" s="17">
+        <f t="shared" si="6"/>
+        <v>1.7473661116001722</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20">
+      <c r="A8">
         <f t="shared" si="0"/>
         <v>0.52359877559829882</v>
       </c>
-      <c r="B7">
+      <c r="B8" s="11">
         <v>30</v>
       </c>
-      <c r="C7">
+      <c r="C8" s="7">
         <f t="shared" si="1"/>
         <v>0.57735026918962573</v>
       </c>
-      <c r="D7">
+      <c r="D8" s="15">
         <f t="shared" si="2"/>
         <v>747.66859860056536</v>
       </c>
-      <c r="E7">
+      <c r="E8" s="7">
         <v>350</v>
       </c>
-      <c r="F7">
+      <c r="F8" s="15">
         <f t="shared" si="3"/>
         <v>397.66859860056536</v>
       </c>
-      <c r="G7">
+      <c r="G8" s="18">
+        <f t="shared" si="5"/>
+        <v>0.44134185494809841</v>
+      </c>
+      <c r="S8" s="17">
         <f t="shared" si="4"/>
-        <v>1.0044134185494811</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11">
-      <c r="A8">
+        <v>429.0847552567385</v>
+      </c>
+      <c r="T8" s="17">
+        <f t="shared" si="6"/>
+        <v>6.0847552567385037</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20">
+      <c r="A9">
         <f t="shared" si="0"/>
         <v>0.56723200689815712</v>
       </c>
-      <c r="B8">
+      <c r="B9" s="11">
         <v>32.5</v>
       </c>
-      <c r="C8">
+      <c r="C9" s="7">
         <f t="shared" si="1"/>
         <v>0.63707026080749318</v>
       </c>
-      <c r="D8">
+      <c r="D9" s="15">
         <f t="shared" si="2"/>
         <v>825.00598774570369</v>
       </c>
-      <c r="E8">
+      <c r="E9" s="7">
         <v>423</v>
       </c>
-      <c r="F8">
-        <f t="shared" si="3"/>
+      <c r="F9" s="15">
+        <f>D9-E9</f>
         <v>402.00598774570369</v>
       </c>
-      <c r="G8">
+      <c r="G9" s="18">
+        <f t="shared" si="5"/>
+        <v>1.5368600513002528</v>
+      </c>
+      <c r="S9" s="17">
         <f t="shared" si="4"/>
-        <v>1.0153686005130025</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11">
-      <c r="A9">
+        <v>510.84752949260894</v>
+      </c>
+      <c r="T9" s="17">
+        <f t="shared" si="6"/>
+        <v>6.8475294926089418</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20">
+      <c r="A10">
         <f t="shared" si="0"/>
         <v>0.6108652381980153</v>
       </c>
-      <c r="B9">
+      <c r="B10" s="11">
         <v>35</v>
       </c>
-      <c r="C9">
+      <c r="C10" s="7">
         <f t="shared" si="1"/>
         <v>0.70020753820970971</v>
       </c>
-      <c r="D9">
+      <c r="D10" s="15">
         <f t="shared" si="2"/>
         <v>906.76876198157413</v>
       </c>
-      <c r="E9">
+      <c r="E10" s="7">
         <v>504</v>
       </c>
-      <c r="F9">
+      <c r="F10" s="15">
         <f t="shared" si="3"/>
         <v>402.76876198157413</v>
       </c>
-      <c r="G9">
+      <c r="G10" s="18">
+        <f t="shared" si="5"/>
+        <v>1.7295181290384043</v>
+      </c>
+      <c r="S10" s="17">
         <f t="shared" si="4"/>
-        <v>1.0172951812903841</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11">
-      <c r="A10">
+        <v>597.76721694378853</v>
+      </c>
+      <c r="T10" s="17">
+        <f t="shared" si="6"/>
+        <v>11.767216943788526</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20">
+      <c r="A11">
         <f t="shared" si="0"/>
         <v>0.6544984694978736</v>
       </c>
-      <c r="B10">
+      <c r="B11" s="11">
         <v>37.5</v>
       </c>
-      <c r="C10">
+      <c r="C11" s="7">
         <f t="shared" si="1"/>
         <v>0.76732698797896037</v>
       </c>
-      <c r="D10">
+      <c r="D11" s="15">
         <f t="shared" si="2"/>
         <v>993.68844943275371</v>
       </c>
-      <c r="E10">
+      <c r="E11" s="7">
         <v>586</v>
       </c>
-      <c r="F10">
+      <c r="F11" s="15">
         <f t="shared" si="3"/>
         <v>407.68844943275371</v>
       </c>
-      <c r="G10">
+      <c r="G11" s="18">
+        <f t="shared" si="5"/>
+        <v>2.9721106063985827</v>
+      </c>
+      <c r="S11" s="17">
         <f t="shared" si="4"/>
-        <v>1.0297211060639859</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11">
-      <c r="A11">
+        <v>690.71278988561221</v>
+      </c>
+      <c r="T11" s="17">
+        <f t="shared" si="6"/>
+        <v>14.71278988561221</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20">
+      <c r="A12">
         <f t="shared" si="0"/>
         <v>0.69813170079773179</v>
       </c>
-      <c r="B11">
+      <c r="B12" s="11">
         <v>40</v>
       </c>
-      <c r="C11">
+      <c r="C12" s="7">
         <f t="shared" si="1"/>
         <v>0.83909963117727993</v>
       </c>
-      <c r="D11">
+      <c r="D12" s="15">
         <f t="shared" si="2"/>
         <v>1086.6340223745774</v>
       </c>
-      <c r="E11">
+      <c r="E12" s="7">
         <v>676</v>
       </c>
-      <c r="F11">
+      <c r="F12" s="15">
         <f t="shared" si="3"/>
         <v>410.6340223745774</v>
       </c>
-      <c r="G11">
+      <c r="G12" s="18">
+        <f t="shared" si="5"/>
+        <v>3.7160901407383533</v>
+      </c>
+      <c r="S12" s="17">
         <f t="shared" si="4"/>
-        <v>1.0371609014073835</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11">
-      <c r="A12">
+        <v>770.10200487673751</v>
+      </c>
+      <c r="T12" s="17">
+        <f t="shared" si="6"/>
+        <v>21.10200487673751</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20">
+      <c r="A13">
         <f t="shared" si="0"/>
         <v>0.73303828583761843</v>
       </c>
-      <c r="B12">
+      <c r="B13" s="11">
         <v>42</v>
       </c>
-      <c r="C12">
+      <c r="C13" s="7">
         <f t="shared" si="1"/>
         <v>0.90040404429783993</v>
       </c>
-      <c r="D12">
+      <c r="D13" s="15">
         <f t="shared" si="2"/>
         <v>1166.0232373657027</v>
       </c>
-      <c r="E12">
+      <c r="E13" s="7">
         <v>749</v>
       </c>
-      <c r="F12">
+      <c r="F13" s="15">
         <f t="shared" si="3"/>
         <v>417.0232373657027</v>
       </c>
-      <c r="G12">
-        <f t="shared" si="4"/>
-        <v>1.0532984925917699</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11">
-      <c r="A13">
+      <c r="G13" s="18">
+        <f t="shared" si="5"/>
+        <v>5.3298492591769877</v>
+      </c>
+      <c r="S13" s="17">
+        <f>D14-$D$3</f>
+        <v>899.07876751103458</v>
+      </c>
+      <c r="T13" s="17">
+        <f t="shared" si="6"/>
+        <v>26.078767511034584</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" ht="15.75" thickBot="1">
+      <c r="A14">
         <f t="shared" si="0"/>
         <v>0.78539816339744828</v>
       </c>
-      <c r="B13">
+      <c r="B14" s="13">
         <v>45</v>
       </c>
-      <c r="C13">
+      <c r="C14" s="14">
         <f t="shared" si="1"/>
         <v>0.99999999999999989</v>
       </c>
-      <c r="D13">
+      <c r="D14" s="16">
         <f t="shared" si="2"/>
         <v>1294.9999999999998</v>
       </c>
-      <c r="E13">
+      <c r="E14" s="14">
         <v>873</v>
       </c>
-      <c r="F13">
+      <c r="F14" s="16">
         <f t="shared" si="3"/>
         <v>421.99999999999977</v>
       </c>
-      <c r="G13">
-        <f t="shared" si="4"/>
-        <v>1.065868575289812</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11">
-      <c r="D16">
-        <f>D2/$D$2</f>
-        <v>1</v>
-      </c>
-      <c r="F16">
-        <f>F2/$D$2</f>
-        <v>1</v>
-      </c>
+      <c r="G14" s="18">
+        <f t="shared" si="5"/>
+        <v>6.5868575289812048</v>
+      </c>
+      <c r="S14" s="17"/>
     </row>
     <row r="17" spans="2:6">
       <c r="D17">
-        <f>D5/$D$2</f>
-        <v>1.5252236246954847</v>
+        <f>D3/$D$3</f>
+        <v>1</v>
       </c>
       <c r="F17">
-        <f>F5/$D$2</f>
-        <v>1.0074438665570686</v>
+        <f>F3/$D$3</f>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="2:6">
       <c r="D18">
-        <f>D9/$D$2</f>
-        <v>2.2902756598355629</v>
+        <f>D6/$D$3</f>
+        <v>1.5252236246954847</v>
       </c>
       <c r="F18">
-        <f>F9/$D$2</f>
-        <v>1.0172951812903841</v>
+        <f>F6/$D$3</f>
+        <v>1.0074438665570686</v>
       </c>
     </row>
     <row r="19" spans="2:6">
       <c r="D19">
-        <f>D11/$D$2</f>
-        <v>2.7445712258052826</v>
+        <f>D10/$D$3</f>
+        <v>2.2902756598355629</v>
       </c>
       <c r="F19">
-        <f>F11/$D$2</f>
-        <v>1.0371609014073835</v>
+        <f>F10/$D$3</f>
+        <v>1.0172951812903841</v>
       </c>
     </row>
     <row r="20" spans="2:6">
       <c r="D20">
-        <f>D13/$D$2</f>
+        <f>D12/$D$3</f>
+        <v>2.7445712258052826</v>
+      </c>
+      <c r="F20">
+        <f>F12/$D$3</f>
+        <v>1.0371609014073835</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6">
+      <c r="D21">
+        <f>D14/$D$3</f>
         <v>3.27085261848414</v>
       </c>
-      <c r="F20">
-        <f>F13/$D$2</f>
+      <c r="F21">
+        <f>F14/$D$3</f>
         <v>1.065868575289812</v>
       </c>
     </row>
-    <row r="21" spans="2:6" ht="15.75" customHeight="1"/>
     <row r="22" spans="2:6" ht="15.75" customHeight="1"/>
     <row r="23" spans="2:6" ht="15.75" customHeight="1"/>
     <row r="24" spans="2:6" ht="15.75" customHeight="1"/>
     <row r="25" spans="2:6" ht="15.75" customHeight="1"/>
-    <row r="26" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B26" s="3" t="s">
+    <row r="26" spans="2:6" ht="15.75" customHeight="1"/>
+    <row r="27" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B27" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="4"/>
-    </row>
-    <row r="27" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B27" s="4"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
     </row>
     <row r="28" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
     </row>
     <row r="29" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B29" s="4"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="4"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
     </row>
     <row r="30" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B30" s="4"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="4"/>
-      <c r="E30" s="4"/>
-      <c r="F30" s="4"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
     </row>
     <row r="31" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B31" s="4"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="4"/>
-      <c r="E31" s="4"/>
-      <c r="F31" s="4"/>
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5"/>
     </row>
     <row r="32" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B32" s="4"/>
-      <c r="C32" s="4"/>
-      <c r="D32" s="4"/>
-      <c r="E32" s="4"/>
-      <c r="F32" s="4"/>
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
     </row>
     <row r="33" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B33" s="4"/>
-      <c r="C33" s="4"/>
-      <c r="D33" s="4"/>
-      <c r="E33" s="4"/>
-      <c r="F33" s="4"/>
+      <c r="B33" s="5"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
     </row>
     <row r="34" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B34" s="4"/>
-      <c r="C34" s="4"/>
-      <c r="D34" s="4"/>
-      <c r="E34" s="4"/>
-      <c r="F34" s="4"/>
+      <c r="B34" s="5"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="5"/>
+      <c r="F34" s="5"/>
     </row>
     <row r="35" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B35" s="4"/>
-      <c r="C35" s="4"/>
-      <c r="D35" s="4"/>
-      <c r="E35" s="4"/>
-      <c r="F35" s="4"/>
-    </row>
-    <row r="36" spans="2:6" ht="15.75" customHeight="1"/>
+      <c r="B35" s="5"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="5"/>
+      <c r="F35" s="5"/>
+    </row>
+    <row r="36" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B36" s="5"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="5"/>
+      <c r="E36" s="5"/>
+      <c r="F36" s="5"/>
+    </row>
     <row r="37" spans="2:6" ht="15.75" customHeight="1"/>
     <row r="38" spans="2:6" ht="15.75" customHeight="1"/>
     <row r="39" spans="2:6" ht="15.75" customHeight="1"/>
@@ -4119,13 +4760,15 @@
     <row r="998" ht="15.75" customHeight="1"/>
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
+    <row r="1001" ht="15.75" customHeight="1"/>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B26:F35"/>
+  <mergeCells count="2">
+    <mergeCell ref="B27:F36"/>
+    <mergeCell ref="B1:G1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -4133,7 +4776,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -4142,8 +4787,9 @@
     <col min="4" max="4" width="15.140625" customWidth="1"/>
     <col min="5" max="5" width="21.85546875" customWidth="1"/>
     <col min="6" max="6" width="19" customWidth="1"/>
-    <col min="7" max="9" width="8.7109375" customWidth="1"/>
-    <col min="10" max="10" width="23.85546875" customWidth="1"/>
+    <col min="7" max="8" width="8.7109375" customWidth="1"/>
+    <col min="9" max="9" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4185,20 +4831,20 @@
         <f t="shared" ref="C2:C12" si="1">TAN(RADIANS(B2))</f>
         <v>0.30573068145866039</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="17">
         <f t="shared" ref="D2:D12" si="2">C2*$K$2</f>
         <v>402.02895567989827</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="17">
         <f t="shared" ref="F2:F12" si="3">D2-E2</f>
         <v>402.02895567989827</v>
       </c>
-      <c r="G2">
-        <f t="shared" ref="G2:G12" si="4">F2/$D$2</f>
-        <v>1</v>
+      <c r="G2" s="6">
+        <f>(F2-$D$2)/$D$2</f>
+        <v>0</v>
       </c>
       <c r="I2">
         <v>10</v>
@@ -4223,20 +4869,20 @@
         <f t="shared" si="1"/>
         <v>0.36397023426620234</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="17">
         <f t="shared" si="2"/>
         <v>478.61265504160701</v>
       </c>
       <c r="E3">
         <v>77</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="17">
         <f t="shared" si="3"/>
         <v>401.61265504160701</v>
       </c>
-      <c r="G3">
-        <f t="shared" si="4"/>
-        <v>0.9989645008589314</v>
+      <c r="G3" s="6">
+        <f t="shared" ref="G3:G12" si="4">(F3-$D$2)/$D$2</f>
+        <v>-1.0354991410686507E-3</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -4251,20 +4897,20 @@
         <f t="shared" si="1"/>
         <v>0.41421356237309503</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="17">
         <f t="shared" si="2"/>
         <v>544.68149913773937</v>
       </c>
       <c r="E4">
         <v>141</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="17">
         <f t="shared" si="3"/>
         <v>403.68149913773937</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="6">
         <f t="shared" si="4"/>
-        <v>1.0041105085454514</v>
+        <v>4.1105085454513175E-3</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -4279,20 +4925,20 @@
         <f t="shared" si="1"/>
         <v>0.46630765815499858</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="17">
         <f t="shared" si="2"/>
         <v>613.18406101463484</v>
       </c>
       <c r="E5">
         <v>209</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="17">
         <f t="shared" si="3"/>
         <v>404.18406101463484</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="6">
         <f t="shared" si="4"/>
-        <v>1.0053605724271575</v>
+        <v>5.3605724271574345E-3</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -4307,20 +4953,20 @@
         <f t="shared" si="1"/>
         <v>0.52056705055174624</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="17">
         <f t="shared" si="2"/>
         <v>684.53393913944399</v>
       </c>
       <c r="E6">
         <v>278</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="17">
         <f t="shared" si="3"/>
         <v>406.53393913944399</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="6">
         <f t="shared" si="4"/>
-        <v>1.0112056193861136</v>
+        <v>1.1205619386113698E-2</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -4335,20 +4981,20 @@
         <f t="shared" si="1"/>
         <v>0.57735026918962573</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="17">
         <f t="shared" si="2"/>
         <v>759.20259189033516</v>
       </c>
       <c r="E7">
         <v>351</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="17">
         <f t="shared" si="3"/>
         <v>408.20259189033516</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="6">
         <f t="shared" si="4"/>
-        <v>1.0153561979136458</v>
+        <v>1.5356197913645871E-2</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -4363,20 +5009,20 @@
         <f t="shared" si="1"/>
         <v>0.63707026080749318</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="17">
         <f t="shared" si="2"/>
         <v>837.73303492207231</v>
       </c>
       <c r="E8">
         <v>427</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="17">
         <f t="shared" si="3"/>
         <v>410.73303492207231</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="6">
         <f t="shared" si="4"/>
-        <v>1.021650378957043</v>
+        <v>2.1650378957042974E-2</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -4391,20 +5037,20 @@
         <f t="shared" si="1"/>
         <v>0.70020753820970971</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="17">
         <f t="shared" si="2"/>
         <v>920.75713174278133</v>
       </c>
       <c r="E9">
         <v>510</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="17">
         <f t="shared" si="3"/>
         <v>410.75713174278133</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="6">
         <f t="shared" si="4"/>
-        <v>1.0217103169798361</v>
+        <v>2.1710316979836053E-2</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -4419,20 +5065,20 @@
         <f t="shared" si="1"/>
         <v>0.76732698797896037</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="17">
         <f t="shared" si="2"/>
         <v>1009.0176954775005</v>
       </c>
       <c r="E10">
         <v>593</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="17">
         <f t="shared" si="3"/>
         <v>416.01769547750052</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="6">
         <f t="shared" si="4"/>
-        <v>1.0347953539165977</v>
+        <v>3.4795353916597743E-2</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -4447,20 +5093,20 @@
         <f t="shared" si="1"/>
         <v>0.83909963117727993</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="17">
         <f t="shared" si="2"/>
         <v>1103.3971036995961</v>
       </c>
       <c r="E11">
         <v>684</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="17">
         <f t="shared" si="3"/>
         <v>419.39710369959607</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="6">
         <f t="shared" si="4"/>
-        <v>1.0432012365634842</v>
+        <v>4.3201236563484222E-2</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -4475,97 +5121,201 @@
         <f t="shared" si="1"/>
         <v>0.90040404429783993</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="17">
         <f t="shared" si="2"/>
         <v>1184.0110252983034</v>
       </c>
       <c r="E12">
         <v>760</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="17">
         <f t="shared" si="3"/>
         <v>424.01102529830337</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="6">
         <f t="shared" si="4"/>
-        <v>1.0546778268277461</v>
-      </c>
-    </row>
-    <row r="21" spans="2:6" ht="15.75" customHeight="1"/>
-    <row r="22" spans="2:6" ht="15.75" customHeight="1"/>
-    <row r="23" spans="2:6" ht="15.75" customHeight="1"/>
-    <row r="24" spans="2:6" ht="15.75" customHeight="1"/>
+        <v>5.4677826827746107E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="15" customHeight="1">
+      <c r="B14" s="17">
+        <f>D2-$D$2</f>
+        <v>0</v>
+      </c>
+      <c r="C14" s="17">
+        <f>B14-E2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="15" customHeight="1">
+      <c r="B15" s="17">
+        <f t="shared" ref="B15:B27" si="5">D3-$D$2</f>
+        <v>76.583699361708739</v>
+      </c>
+      <c r="C15" s="17">
+        <f t="shared" ref="C15:C24" si="6">B15-E3</f>
+        <v>-0.41630063829126129</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="15" customHeight="1">
+      <c r="B16" s="17">
+        <f t="shared" si="5"/>
+        <v>142.65254345784109</v>
+      </c>
+      <c r="C16" s="17">
+        <f t="shared" si="6"/>
+        <v>1.6525434578410909</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" ht="15" customHeight="1">
+      <c r="B17" s="17">
+        <f t="shared" si="5"/>
+        <v>211.15510533473656</v>
+      </c>
+      <c r="C17" s="17">
+        <f t="shared" si="6"/>
+        <v>2.155105334736561</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" ht="15" customHeight="1">
+      <c r="B18" s="17">
+        <f t="shared" si="5"/>
+        <v>282.50498345954571</v>
+      </c>
+      <c r="C18" s="17">
+        <f t="shared" si="6"/>
+        <v>4.5049834595457128</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" ht="15" customHeight="1">
+      <c r="B19" s="17">
+        <f t="shared" si="5"/>
+        <v>357.17363621043688</v>
+      </c>
+      <c r="C19" s="17">
+        <f t="shared" si="6"/>
+        <v>6.1736362104368823</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" ht="15" customHeight="1">
+      <c r="B20" s="17">
+        <f t="shared" si="5"/>
+        <v>435.70407924217403</v>
+      </c>
+      <c r="C20" s="17">
+        <f t="shared" si="6"/>
+        <v>8.7040792421740321</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B21" s="17">
+        <f t="shared" si="5"/>
+        <v>518.72817606288299</v>
+      </c>
+      <c r="C21" s="17">
+        <f t="shared" si="6"/>
+        <v>8.7281760628829943</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B22" s="17">
+        <f t="shared" si="5"/>
+        <v>606.98873979760219</v>
+      </c>
+      <c r="C22" s="17">
+        <f t="shared" si="6"/>
+        <v>13.988739797602193</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B23" s="17">
+        <f t="shared" si="5"/>
+        <v>701.36814801969786</v>
+      </c>
+      <c r="C23" s="17">
+        <f t="shared" si="6"/>
+        <v>17.368148019697855</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B24" s="17">
+        <f t="shared" si="5"/>
+        <v>781.98206961840515</v>
+      </c>
+      <c r="C24" s="17">
+        <f t="shared" si="6"/>
+        <v>21.982069618405149</v>
+      </c>
+    </row>
     <row r="25" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B25" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
+      <c r="B25" s="17"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
     </row>
     <row r="26" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="4"/>
+      <c r="B26" s="17"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
     </row>
     <row r="27" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B27" s="4"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
+      <c r="B27" s="17"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
     </row>
     <row r="28" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
     </row>
     <row r="29" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B29" s="4"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="4"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
     </row>
     <row r="30" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B30" s="4"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="4"/>
-      <c r="E30" s="4"/>
-      <c r="F30" s="4"/>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
     </row>
     <row r="31" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B31" s="4"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="4"/>
-      <c r="E31" s="4"/>
-      <c r="F31" s="4"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
     </row>
     <row r="32" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B32" s="4"/>
-      <c r="C32" s="4"/>
-      <c r="D32" s="4"/>
-      <c r="E32" s="4"/>
-      <c r="F32" s="4"/>
+      <c r="B32" s="3"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
     </row>
     <row r="33" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B33" s="4"/>
-      <c r="C33" s="4"/>
-      <c r="D33" s="4"/>
-      <c r="E33" s="4"/>
-      <c r="F33" s="4"/>
+      <c r="B33" s="3"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
     </row>
     <row r="34" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B34" s="4"/>
-      <c r="C34" s="4"/>
-      <c r="D34" s="4"/>
-      <c r="E34" s="4"/>
-      <c r="F34" s="4"/>
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
     </row>
     <row r="35" spans="2:6" ht="15.75" customHeight="1"/>
     <row r="36" spans="2:6" ht="15.75" customHeight="1"/>
@@ -5534,9 +6284,6 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B25:F34"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
   <drawing r:id="rId1"/>
@@ -5910,76 +6657,76 @@
     <row r="23" spans="2:6" ht="15.75" customHeight="1"/>
     <row r="24" spans="2:6" ht="15.75" customHeight="1"/>
     <row r="25" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B25" s="3" t="s">
+      <c r="B25" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
     </row>
     <row r="26" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="4"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
     </row>
     <row r="27" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B27" s="4"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
     </row>
     <row r="28" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
     </row>
     <row r="29" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B29" s="4"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="4"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
     </row>
     <row r="30" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B30" s="4"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="4"/>
-      <c r="E30" s="4"/>
-      <c r="F30" s="4"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
     </row>
     <row r="31" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B31" s="4"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="4"/>
-      <c r="E31" s="4"/>
-      <c r="F31" s="4"/>
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5"/>
     </row>
     <row r="32" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B32" s="4"/>
-      <c r="C32" s="4"/>
-      <c r="D32" s="4"/>
-      <c r="E32" s="4"/>
-      <c r="F32" s="4"/>
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
     </row>
     <row r="33" spans="2:7" ht="15.75" customHeight="1">
-      <c r="B33" s="4"/>
-      <c r="C33" s="4"/>
-      <c r="D33" s="4"/>
-      <c r="E33" s="4"/>
-      <c r="F33" s="4"/>
+      <c r="B33" s="5"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
     </row>
     <row r="34" spans="2:7" ht="15.75" customHeight="1">
-      <c r="B34" s="4"/>
-      <c r="C34" s="4"/>
-      <c r="D34" s="4"/>
-      <c r="E34" s="4"/>
-      <c r="F34" s="4"/>
+      <c r="B34" s="5"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="5"/>
+      <c r="F34" s="5"/>
     </row>
     <row r="35" spans="2:7" ht="15.75" customHeight="1"/>
     <row r="36" spans="2:7" ht="15.75" customHeight="1"/>
@@ -7020,7 +7767,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="P18" sqref="P18"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Moved todo list to word doc for formatting Work on main paper. especially design section.
</commit_message>
<xml_diff>
--- a/Testing/Relative Positioning/Altitude Relative Measure/Altitude Relative Measure Calculations.xlsx
+++ b/Testing/Relative Positioning/Altitude Relative Measure/Altitude Relative Measure Calculations.xlsx
@@ -1,25 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="630" yWindow="600" windowWidth="27495" windowHeight="13740" activeTab="1"/>
+    <workbookView xWindow="630" yWindow="600" windowWidth="27495" windowHeight="13740" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Az=0 (4-3-18)" sheetId="1" r:id="rId1"/>
     <sheet name="Az=0 Plot with Error bars" sheetId="6" r:id="rId2"/>
-    <sheet name="Az=0 (4-4-18 retest)" sheetId="2" r:id="rId3"/>
-    <sheet name="Az=10 (4-4-18)" sheetId="3" r:id="rId4"/>
-    <sheet name="Az=10 (4-6-18)(angle apparatus)" sheetId="4" r:id="rId5"/>
-    <sheet name="Grid Measurements" sheetId="5" r:id="rId6"/>
+    <sheet name="Az=0 cmd vs cmd-calc" sheetId="7" r:id="rId3"/>
+    <sheet name="Az=0 (4-4-18 retest)" sheetId="2" r:id="rId4"/>
+    <sheet name="Az=10 (4-4-18)" sheetId="3" r:id="rId5"/>
+    <sheet name="Az=10 (4-6-18)(angle apparatus)" sheetId="4" r:id="rId6"/>
+    <sheet name="Grid Measurements" sheetId="5" r:id="rId7"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="37">
   <si>
     <t>TAN</t>
   </si>
@@ -145,6 +146,12 @@
       <t>, DistanceToBoard = 1295mm</t>
     </r>
   </si>
+  <si>
+    <t>Calculated Angle</t>
+  </si>
+  <si>
+    <t>Cmd minus Calc Angle</t>
+  </si>
 </sst>
 </file>
 
@@ -186,7 +193,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -314,22 +321,42 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -339,14 +366,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -449,11 +468,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="145450880"/>
-        <c:axId val="145453056"/>
+        <c:axId val="133976448"/>
+        <c:axId val="133985408"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="145450880"/>
+        <c:axId val="133976448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -487,12 +506,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="145453056"/>
+        <c:crossAx val="133985408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="145453056"/>
+        <c:axId val="133985408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -526,7 +545,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="145450880"/>
+        <c:crossAx val="133976448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -538,7 +557,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -769,11 +787,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="135836032"/>
-        <c:axId val="135837568"/>
+        <c:axId val="165119488"/>
+        <c:axId val="165121408"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="135836032"/>
+        <c:axId val="165119488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -795,19 +813,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="135837568"/>
+        <c:crossAx val="165121408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="135837568"/>
+        <c:axId val="165121408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -835,14 +852,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="135836032"/>
+        <c:crossAx val="165119488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -855,6 +871,228 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Az=0 (4-4-18 retest)'!$B$3:$B$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>22.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>27.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>32.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>37.5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>45</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Az=0 (4-4-18 retest)'!$I$3:$I$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>-4.9868769295358106E-5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.2599586120112036E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-1.8377251557794239E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-0.10724365958140325</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-7.7136005254676121E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-5.8057469727032185E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-0.19194047953175186</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-0.20383212795654515</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-0.32916294883163744</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-0.38416899017933304</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-0.51984098395346479</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-0.58278822910520489</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="165141888"/>
+        <c:axId val="165156352"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="165141888"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="46"/>
+          <c:min val="15"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Command</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Angle [deg]</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="165156352"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="165156352"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="5.000000000000001E-2"/>
+          <c:min val="-0.60000000000000009"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Command Angle minus</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Calculated Angle [deg]</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="165141888"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -989,11 +1227,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="145969920"/>
-        <c:axId val="145971456"/>
+        <c:axId val="165303424"/>
+        <c:axId val="165305344"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="145969920"/>
+        <c:axId val="165303424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1027,12 +1265,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="145971456"/>
+        <c:crossAx val="165305344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="145971456"/>
+        <c:axId val="165305344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1066,7 +1304,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="145969920"/>
+        <c:crossAx val="165303424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1078,256 +1316,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="zero"/>
-    <c:showDLblsOverMax val="1"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="1"/>
-  <c:style val="2"/>
-  <c:chart>
-    <c:autoTitleDeleted val="1"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:ln w="47625">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="7"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="4F81BD"/>
-              </a:solidFill>
-              <a:ln cmpd="sng">
-                <a:solidFill>
-                  <a:srgbClr val="4F81BD"/>
-                </a:solidFill>
-              </a:ln>
-            </c:spPr>
-          </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-              </a:ln>
-            </c:spPr>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="1"/>
-            <c:dispEq val="0"/>
-            <c:trendlineLbl>
-              <c:layout/>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-            </c:trendlineLbl>
-          </c:trendline>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'Az=10 (4-4-18)'!$D$2:$D$12</c:f>
-              <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>402.02895567989827</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>478.61265504160701</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>544.68149913773937</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>613.18406101463484</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>684.53393913944399</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>759.20259189033516</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>837.73303492207231</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>920.75713174278133</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1009.0176954775005</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1103.3971036995961</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1184.0110252983034</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'Az=10 (4-4-18)'!$G$2:$G$12</c:f>
-              <c:numCache>
-                <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>-1.0354991410686507E-3</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4.1105085454513175E-3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5.3605724271574345E-3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.1205619386113698E-2</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.5356197913645871E-2</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2.1650378957042974E-2</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2.1710316979836053E-2</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>3.4795353916597743E-2</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>4.3201236563484222E-2</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>5.4677826827746107E-2</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="146017280"/>
-        <c:axId val="146019072"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="146017280"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
-        <c:majorTickMark val="cross"/>
-        <c:minorTickMark val="cross"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="47625">
-            <a:noFill/>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr lvl="0">
-              <a:defRPr b="0"/>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="146019072"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="146019072"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:srgbClr val="B7B7B7"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
-        <c:majorTickMark val="cross"/>
-        <c:minorTickMark val="cross"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="47625">
-            <a:noFill/>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr lvl="0">
-              <a:defRPr b="0"/>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="146017280"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:solidFill>
-          <a:srgbClr val="FFFFFF"/>
-        </a:solidFill>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1389,15 +1377,14 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="0"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Az=10 (4-6-18)(angle apparatus)'!$D$2:$D$12</c:f>
+              <c:f>'Az=10 (4-4-18)'!$D$2:$D$12</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>402.02895567989827</c:v>
@@ -1437,42 +1424,42 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Az=10 (4-6-18)(angle apparatus)'!$G$2:$G$12</c:f>
+              <c:f>'Az=10 (4-4-18)'!$G$2:$G$12</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.9989645008589314</c:v>
+                  <c:v>-1.0354991410686507E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.0041105085454514</c:v>
+                  <c:v>4.1105085454513175E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.0053605724271575</c:v>
+                  <c:v>5.3605724271574345E-3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.0112056193861136</c:v>
+                  <c:v>1.1205619386113698E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.0153561979136458</c:v>
+                  <c:v>1.5356197913645871E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.021650378957043</c:v>
+                  <c:v>2.1650378957042974E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.0217103169798361</c:v>
+                  <c:v>2.1710316979836053E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.0347953539165977</c:v>
+                  <c:v>3.4795353916597743E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.0432012365634842</c:v>
+                  <c:v>4.3201236563484222E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.0546778268277461</c:v>
+                  <c:v>5.4677826827746107E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1487,11 +1474,258 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="146086912"/>
-        <c:axId val="146092800"/>
+        <c:axId val="165350784"/>
+        <c:axId val="165364864"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="146086912"/>
+        <c:axId val="165350784"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="cross"/>
+        <c:minorTickMark val="cross"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="47625">
+            <a:noFill/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="165364864"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="165364864"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="B7B7B7"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+        <c:majorTickMark val="cross"/>
+        <c:minorTickMark val="cross"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="47625">
+            <a:noFill/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="165350784"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="1"/>
+  <c:style val="2"/>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="47625">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="7"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="4F81BD"/>
+              </a:solidFill>
+              <a:ln cmpd="sng">
+                <a:solidFill>
+                  <a:srgbClr val="4F81BD"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="0"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Az=10 (4-6-18)(angle apparatus)'!$D$2:$D$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>402.02895567989827</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>478.61265504160701</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>544.68149913773937</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>613.18406101463484</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>684.53393913944399</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>759.20259189033516</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>837.73303492207231</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>920.75713174278133</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1009.0176954775005</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1103.3971036995961</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1184.0110252983034</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Az=10 (4-6-18)(angle apparatus)'!$G$2:$G$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.9989645008589314</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0041105085454514</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0053605724271575</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.0112056193861136</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.0153561979136458</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.021650378957043</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.0217103169798361</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.0347953539165977</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.0432012365634842</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.0546778268277461</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="165402880"/>
+        <c:axId val="165404672"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="165402880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1525,12 +1759,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="146092800"/>
+        <c:crossAx val="165404672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="146092800"/>
+        <c:axId val="165404672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1564,7 +1798,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="146086912"/>
+        <c:crossAx val="165402880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1576,7 +1810,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1595,7 +1828,18 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" workbookViewId="0"/>
+    <sheetView zoomScale="115" workbookViewId="0"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1636,6 +1880,33 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8671034" cy="6293069"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
     <xdr:ext cx="8671560" cy="6294120"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1659,7 +1930,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
@@ -1689,7 +1960,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
@@ -1719,7 +1990,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
@@ -3186,7 +3457,7 @@
   <dimension ref="A1:T1001"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T3" sqref="T3"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -3197,46 +3468,54 @@
     <col min="4" max="4" width="34" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="31.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="27.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="26" width="8.7109375" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" customWidth="1"/>
+    <col min="8" max="8" width="16" bestFit="1" customWidth="1"/>
+    <col min="9" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" s="3" customFormat="1" ht="15" customHeight="1">
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="10"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="21"/>
     </row>
     <row r="2" spans="1:20">
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="G2" s="8" t="s">
         <v>33</v>
+      </c>
+      <c r="H2" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="I2" s="16" t="s">
+        <v>36</v>
       </c>
       <c r="K2" t="s">
         <v>9</v>
       </c>
-      <c r="S2" s="17">
+      <c r="S2" s="13">
         <f>D3-$D$3</f>
         <v>0</v>
       </c>
-      <c r="T2" s="17">
+      <c r="T2" s="13">
         <f>S2-E3</f>
         <v>0</v>
       </c>
@@ -3246,36 +3525,44 @@
         <f t="shared" ref="A3:A14" si="0">RADIANS(B3)</f>
         <v>0.29670597283903605</v>
       </c>
-      <c r="B3" s="11">
+      <c r="B3" s="7">
         <v>17</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3" s="6">
         <f t="shared" ref="C3:C14" si="1">TAN(RADIANS(B3))</f>
         <v>0.30573068145866039</v>
       </c>
-      <c r="D3" s="15">
+      <c r="D3" s="11">
         <f t="shared" ref="D3:D14" si="2">C3*$K$3</f>
         <v>395.92123248896519</v>
       </c>
-      <c r="E3" s="7">
+      <c r="E3" s="6">
         <v>0</v>
       </c>
-      <c r="F3" s="15">
+      <c r="F3" s="11">
         <f t="shared" ref="F3:F14" si="3">D3-E3</f>
         <v>395.92123248896519</v>
       </c>
-      <c r="G3" s="18">
+      <c r="G3" s="14">
         <f>(F3-$D$3)/$D$3*100</f>
         <v>0</v>
       </c>
+      <c r="H3">
+        <f>DEGREES(ATAN((E3+395.92)/1295))</f>
+        <v>16.999950131230705</v>
+      </c>
+      <c r="I3">
+        <f>H3-B3</f>
+        <v>-4.9868769295358106E-5</v>
+      </c>
       <c r="K3">
         <v>1295</v>
       </c>
-      <c r="S3" s="17">
-        <f t="shared" ref="S3:S14" si="4">D4-$D$3</f>
+      <c r="S3" s="13">
+        <f t="shared" ref="S3:S12" si="4">D4-$D$3</f>
         <v>75.420220885766867</v>
       </c>
-      <c r="T3" s="17">
+      <c r="T3" s="13">
         <f>S3-E4</f>
         <v>-0.57977911423313344</v>
       </c>
@@ -3285,34 +3572,42 @@
         <f t="shared" si="0"/>
         <v>0.3490658503988659</v>
       </c>
-      <c r="B4" s="11">
+      <c r="B4" s="7">
         <v>20</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="6">
         <f t="shared" si="1"/>
         <v>0.36397023426620234</v>
       </c>
-      <c r="D4" s="15">
+      <c r="D4" s="11">
         <f t="shared" si="2"/>
         <v>471.34145337473205</v>
       </c>
-      <c r="E4" s="7">
+      <c r="E4" s="6">
         <v>76</v>
       </c>
-      <c r="F4" s="15">
+      <c r="F4" s="11">
         <f t="shared" si="3"/>
         <v>395.34145337473205</v>
       </c>
-      <c r="G4" s="18">
+      <c r="G4" s="14">
         <f t="shared" ref="G4:G14" si="5">(F4-$D$3)/$D$3*100</f>
         <v>-0.14643799489821313</v>
       </c>
-      <c r="S4" s="17">
+      <c r="H4" s="4">
+        <f t="shared" ref="H4:H14" si="6">DEGREES(ATAN((E4+395.92)/1295))</f>
+        <v>20.022599586120112</v>
+      </c>
+      <c r="I4" s="4">
+        <f t="shared" ref="I4:I14" si="7">H4-B4</f>
+        <v>2.2599586120112036E-2</v>
+      </c>
+      <c r="S4" s="13">
         <f t="shared" si="4"/>
         <v>140.48533078419291</v>
       </c>
-      <c r="T4" s="17">
-        <f t="shared" ref="T3:T13" si="6">S4-E5</f>
+      <c r="T4" s="13">
+        <f t="shared" ref="T4:T13" si="8">S4-E5</f>
         <v>0.48533078419291087</v>
       </c>
     </row>
@@ -3321,34 +3616,42 @@
         <f t="shared" si="0"/>
         <v>0.39269908169872414</v>
       </c>
-      <c r="B5" s="11">
+      <c r="B5" s="7">
         <v>22.5</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="6">
         <f t="shared" si="1"/>
         <v>0.41421356237309503</v>
       </c>
-      <c r="D5" s="15">
+      <c r="D5" s="11">
         <f t="shared" si="2"/>
         <v>536.4065632731581</v>
       </c>
-      <c r="E5" s="7">
+      <c r="E5" s="6">
         <v>140</v>
       </c>
-      <c r="F5" s="15">
+      <c r="F5" s="11">
         <f t="shared" si="3"/>
         <v>396.4065632731581</v>
       </c>
-      <c r="G5" s="18">
+      <c r="G5" s="14">
         <f t="shared" si="5"/>
         <v>0.12258266149099181</v>
       </c>
-      <c r="S5" s="17">
+      <c r="H5" s="4">
+        <f t="shared" si="6"/>
+        <v>22.481622748442206</v>
+      </c>
+      <c r="I5" s="4">
+        <f t="shared" si="7"/>
+        <v>-1.8377251557794239E-2</v>
+      </c>
+      <c r="S5" s="13">
         <f t="shared" si="4"/>
         <v>207.94718482175801</v>
       </c>
-      <c r="T5" s="17">
-        <f t="shared" si="6"/>
+      <c r="T5" s="13">
+        <f t="shared" si="8"/>
         <v>2.9471848217580146</v>
       </c>
     </row>
@@ -3357,34 +3660,42 @@
         <f t="shared" si="0"/>
         <v>0.43633231299858238</v>
       </c>
-      <c r="B6" s="11">
+      <c r="B6" s="7">
         <v>25</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="6">
         <f t="shared" si="1"/>
         <v>0.46630765815499858</v>
       </c>
-      <c r="D6" s="15">
+      <c r="D6" s="11">
         <f t="shared" si="2"/>
         <v>603.8684173107232</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E6" s="6">
         <v>205</v>
       </c>
-      <c r="F6" s="15">
+      <c r="F6" s="11">
         <f t="shared" si="3"/>
         <v>398.8684173107232</v>
       </c>
-      <c r="G6" s="18">
+      <c r="G6" s="14">
         <f t="shared" si="5"/>
         <v>0.74438665570686613</v>
       </c>
-      <c r="S6" s="17">
+      <c r="H6" s="4">
+        <f t="shared" si="6"/>
+        <v>24.892756340418597</v>
+      </c>
+      <c r="I6" s="4">
+        <f t="shared" si="7"/>
+        <v>-0.10724365958140325</v>
+      </c>
+      <c r="S6" s="13">
         <f t="shared" si="4"/>
         <v>278.21309797554613</v>
       </c>
-      <c r="T6" s="17">
-        <f t="shared" si="6"/>
+      <c r="T6" s="13">
+        <f t="shared" si="8"/>
         <v>2.213097975546134</v>
       </c>
     </row>
@@ -3393,34 +3704,42 @@
         <f t="shared" si="0"/>
         <v>0.47996554429844063</v>
       </c>
-      <c r="B7" s="11">
+      <c r="B7" s="7">
         <v>27.5</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="6">
         <f t="shared" si="1"/>
         <v>0.52056705055174624</v>
       </c>
-      <c r="D7" s="15">
+      <c r="D7" s="11">
         <f t="shared" si="2"/>
         <v>674.13433046451132</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="6">
         <v>276</v>
       </c>
-      <c r="F7" s="15">
+      <c r="F7" s="11">
         <f t="shared" si="3"/>
         <v>398.13433046451132</v>
       </c>
-      <c r="G7" s="18">
+      <c r="G7" s="14">
         <f t="shared" si="5"/>
         <v>0.55897430951946125</v>
       </c>
-      <c r="S7" s="17">
+      <c r="H7" s="4">
+        <f t="shared" si="6"/>
+        <v>27.422863994745324</v>
+      </c>
+      <c r="I7" s="4">
+        <f t="shared" si="7"/>
+        <v>-7.7136005254676121E-2</v>
+      </c>
+      <c r="S7" s="13">
         <f t="shared" si="4"/>
         <v>351.74736611160017</v>
       </c>
-      <c r="T7" s="17">
-        <f t="shared" si="6"/>
+      <c r="T7" s="13">
+        <f t="shared" si="8"/>
         <v>1.7473661116001722</v>
       </c>
     </row>
@@ -3429,34 +3748,42 @@
         <f t="shared" si="0"/>
         <v>0.52359877559829882</v>
       </c>
-      <c r="B8" s="11">
+      <c r="B8" s="7">
         <v>30</v>
       </c>
-      <c r="C8" s="7">
+      <c r="C8" s="6">
         <f t="shared" si="1"/>
         <v>0.57735026918962573</v>
       </c>
-      <c r="D8" s="15">
+      <c r="D8" s="11">
         <f t="shared" si="2"/>
         <v>747.66859860056536</v>
       </c>
-      <c r="E8" s="7">
+      <c r="E8" s="6">
         <v>350</v>
       </c>
-      <c r="F8" s="15">
+      <c r="F8" s="11">
         <f t="shared" si="3"/>
         <v>397.66859860056536</v>
       </c>
-      <c r="G8" s="18">
+      <c r="G8" s="14">
         <f t="shared" si="5"/>
         <v>0.44134185494809841</v>
       </c>
-      <c r="S8" s="17">
+      <c r="H8" s="4">
+        <f t="shared" si="6"/>
+        <v>29.941942530272968</v>
+      </c>
+      <c r="I8" s="4">
+        <f t="shared" si="7"/>
+        <v>-5.8057469727032185E-2</v>
+      </c>
+      <c r="S8" s="13">
         <f t="shared" si="4"/>
         <v>429.0847552567385</v>
       </c>
-      <c r="T8" s="17">
-        <f t="shared" si="6"/>
+      <c r="T8" s="13">
+        <f t="shared" si="8"/>
         <v>6.0847552567385037</v>
       </c>
     </row>
@@ -3465,34 +3792,42 @@
         <f t="shared" si="0"/>
         <v>0.56723200689815712</v>
       </c>
-      <c r="B9" s="11">
+      <c r="B9" s="7">
         <v>32.5</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C9" s="6">
         <f t="shared" si="1"/>
         <v>0.63707026080749318</v>
       </c>
-      <c r="D9" s="15">
+      <c r="D9" s="11">
         <f t="shared" si="2"/>
         <v>825.00598774570369</v>
       </c>
-      <c r="E9" s="7">
+      <c r="E9" s="6">
         <v>423</v>
       </c>
-      <c r="F9" s="15">
+      <c r="F9" s="11">
         <f>D9-E9</f>
         <v>402.00598774570369</v>
       </c>
-      <c r="G9" s="18">
+      <c r="G9" s="14">
         <f t="shared" si="5"/>
         <v>1.5368600513002528</v>
       </c>
-      <c r="S9" s="17">
+      <c r="H9" s="4">
+        <f t="shared" si="6"/>
+        <v>32.308059520468248</v>
+      </c>
+      <c r="I9" s="4">
+        <f t="shared" si="7"/>
+        <v>-0.19194047953175186</v>
+      </c>
+      <c r="S9" s="13">
         <f t="shared" si="4"/>
         <v>510.84752949260894</v>
       </c>
-      <c r="T9" s="17">
-        <f t="shared" si="6"/>
+      <c r="T9" s="13">
+        <f t="shared" si="8"/>
         <v>6.8475294926089418</v>
       </c>
     </row>
@@ -3501,34 +3836,42 @@
         <f t="shared" si="0"/>
         <v>0.6108652381980153</v>
       </c>
-      <c r="B10" s="11">
+      <c r="B10" s="7">
         <v>35</v>
       </c>
-      <c r="C10" s="7">
+      <c r="C10" s="6">
         <f t="shared" si="1"/>
         <v>0.70020753820970971</v>
       </c>
-      <c r="D10" s="15">
+      <c r="D10" s="11">
         <f t="shared" si="2"/>
         <v>906.76876198157413</v>
       </c>
-      <c r="E10" s="7">
+      <c r="E10" s="6">
         <v>504</v>
       </c>
-      <c r="F10" s="15">
+      <c r="F10" s="11">
         <f t="shared" si="3"/>
         <v>402.76876198157413</v>
       </c>
-      <c r="G10" s="18">
+      <c r="G10" s="14">
         <f t="shared" si="5"/>
         <v>1.7295181290384043</v>
       </c>
-      <c r="S10" s="17">
+      <c r="H10" s="4">
+        <f t="shared" si="6"/>
+        <v>34.796167872043455</v>
+      </c>
+      <c r="I10" s="4">
+        <f t="shared" si="7"/>
+        <v>-0.20383212795654515</v>
+      </c>
+      <c r="S10" s="13">
         <f t="shared" si="4"/>
         <v>597.76721694378853</v>
       </c>
-      <c r="T10" s="17">
-        <f t="shared" si="6"/>
+      <c r="T10" s="13">
+        <f t="shared" si="8"/>
         <v>11.767216943788526</v>
       </c>
     </row>
@@ -3537,34 +3880,42 @@
         <f t="shared" si="0"/>
         <v>0.6544984694978736</v>
       </c>
-      <c r="B11" s="11">
+      <c r="B11" s="7">
         <v>37.5</v>
       </c>
-      <c r="C11" s="7">
+      <c r="C11" s="6">
         <f t="shared" si="1"/>
         <v>0.76732698797896037</v>
       </c>
-      <c r="D11" s="15">
+      <c r="D11" s="11">
         <f t="shared" si="2"/>
         <v>993.68844943275371</v>
       </c>
-      <c r="E11" s="7">
+      <c r="E11" s="6">
         <v>586</v>
       </c>
-      <c r="F11" s="15">
+      <c r="F11" s="11">
         <f t="shared" si="3"/>
         <v>407.68844943275371</v>
       </c>
-      <c r="G11" s="18">
+      <c r="G11" s="14">
         <f t="shared" si="5"/>
         <v>2.9721106063985827</v>
       </c>
-      <c r="S11" s="17">
+      <c r="H11" s="4">
+        <f t="shared" si="6"/>
+        <v>37.170837051168363</v>
+      </c>
+      <c r="I11" s="4">
+        <f t="shared" si="7"/>
+        <v>-0.32916294883163744</v>
+      </c>
+      <c r="S11" s="13">
         <f t="shared" si="4"/>
         <v>690.71278988561221</v>
       </c>
-      <c r="T11" s="17">
-        <f t="shared" si="6"/>
+      <c r="T11" s="13">
+        <f t="shared" si="8"/>
         <v>14.71278988561221</v>
       </c>
     </row>
@@ -3573,34 +3924,42 @@
         <f t="shared" si="0"/>
         <v>0.69813170079773179</v>
       </c>
-      <c r="B12" s="11">
+      <c r="B12" s="7">
         <v>40</v>
       </c>
-      <c r="C12" s="7">
+      <c r="C12" s="6">
         <f t="shared" si="1"/>
         <v>0.83909963117727993</v>
       </c>
-      <c r="D12" s="15">
+      <c r="D12" s="11">
         <f t="shared" si="2"/>
         <v>1086.6340223745774</v>
       </c>
-      <c r="E12" s="7">
+      <c r="E12" s="6">
         <v>676</v>
       </c>
-      <c r="F12" s="15">
+      <c r="F12" s="11">
         <f t="shared" si="3"/>
         <v>410.6340223745774</v>
       </c>
-      <c r="G12" s="18">
+      <c r="G12" s="14">
         <f t="shared" si="5"/>
         <v>3.7160901407383533</v>
       </c>
-      <c r="S12" s="17">
+      <c r="H12" s="4">
+        <f t="shared" si="6"/>
+        <v>39.615831009820667</v>
+      </c>
+      <c r="I12" s="4">
+        <f t="shared" si="7"/>
+        <v>-0.38416899017933304</v>
+      </c>
+      <c r="S12" s="13">
         <f t="shared" si="4"/>
         <v>770.10200487673751</v>
       </c>
-      <c r="T12" s="17">
-        <f t="shared" si="6"/>
+      <c r="T12" s="13">
+        <f t="shared" si="8"/>
         <v>21.10200487673751</v>
       </c>
     </row>
@@ -3609,34 +3968,42 @@
         <f t="shared" si="0"/>
         <v>0.73303828583761843</v>
       </c>
-      <c r="B13" s="11">
+      <c r="B13" s="7">
         <v>42</v>
       </c>
-      <c r="C13" s="7">
+      <c r="C13" s="6">
         <f t="shared" si="1"/>
         <v>0.90040404429783993</v>
       </c>
-      <c r="D13" s="15">
+      <c r="D13" s="11">
         <f t="shared" si="2"/>
         <v>1166.0232373657027</v>
       </c>
-      <c r="E13" s="7">
+      <c r="E13" s="6">
         <v>749</v>
       </c>
-      <c r="F13" s="15">
+      <c r="F13" s="11">
         <f t="shared" si="3"/>
         <v>417.0232373657027</v>
       </c>
-      <c r="G13" s="18">
+      <c r="G13" s="14">
         <f t="shared" si="5"/>
         <v>5.3298492591769877</v>
       </c>
-      <c r="S13" s="17">
+      <c r="H13" s="4">
+        <f t="shared" si="6"/>
+        <v>41.480159016046535</v>
+      </c>
+      <c r="I13" s="4">
+        <f t="shared" si="7"/>
+        <v>-0.51984098395346479</v>
+      </c>
+      <c r="S13" s="13">
         <f>D14-$D$3</f>
         <v>899.07876751103458</v>
       </c>
-      <c r="T13" s="17">
-        <f t="shared" si="6"/>
+      <c r="T13" s="13">
+        <f t="shared" si="8"/>
         <v>26.078767511034584</v>
       </c>
     </row>
@@ -3645,29 +4012,37 @@
         <f t="shared" si="0"/>
         <v>0.78539816339744828</v>
       </c>
-      <c r="B14" s="13">
+      <c r="B14" s="9">
         <v>45</v>
       </c>
-      <c r="C14" s="14">
+      <c r="C14" s="10">
         <f t="shared" si="1"/>
         <v>0.99999999999999989</v>
       </c>
-      <c r="D14" s="16">
+      <c r="D14" s="12">
         <f t="shared" si="2"/>
         <v>1294.9999999999998</v>
       </c>
-      <c r="E14" s="14">
+      <c r="E14" s="10">
         <v>873</v>
       </c>
-      <c r="F14" s="16">
+      <c r="F14" s="12">
         <f t="shared" si="3"/>
         <v>421.99999999999977</v>
       </c>
-      <c r="G14" s="18">
+      <c r="G14" s="14">
         <f t="shared" si="5"/>
         <v>6.5868575289812048</v>
       </c>
-      <c r="S14" s="17"/>
+      <c r="H14" s="4">
+        <f t="shared" si="6"/>
+        <v>44.417211770894795</v>
+      </c>
+      <c r="I14" s="4">
+        <f t="shared" si="7"/>
+        <v>-0.58278822910520489</v>
+      </c>
+      <c r="S14" s="13"/>
     </row>
     <row r="17" spans="2:6">
       <c r="D17">
@@ -3725,76 +4100,76 @@
     <row r="25" spans="2:6" ht="15.75" customHeight="1"/>
     <row r="26" spans="2:6" ht="15.75" customHeight="1"/>
     <row r="27" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B27" s="4" t="s">
+      <c r="B27" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="C27" s="5"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="5"/>
-      <c r="F27" s="5"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
     </row>
     <row r="28" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B28" s="5"/>
-      <c r="C28" s="5"/>
-      <c r="D28" s="5"/>
-      <c r="E28" s="5"/>
-      <c r="F28" s="5"/>
+      <c r="B28" s="18"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
     </row>
     <row r="29" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B29" s="5"/>
-      <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="5"/>
-      <c r="F29" s="5"/>
+      <c r="B29" s="18"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="18"/>
     </row>
     <row r="30" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B30" s="5"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="5"/>
-      <c r="E30" s="5"/>
-      <c r="F30" s="5"/>
+      <c r="B30" s="18"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="18"/>
     </row>
     <row r="31" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B31" s="5"/>
-      <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
-      <c r="E31" s="5"/>
-      <c r="F31" s="5"/>
+      <c r="B31" s="18"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="18"/>
     </row>
     <row r="32" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B32" s="5"/>
-      <c r="C32" s="5"/>
-      <c r="D32" s="5"/>
-      <c r="E32" s="5"/>
-      <c r="F32" s="5"/>
+      <c r="B32" s="18"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="18"/>
     </row>
     <row r="33" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B33" s="5"/>
-      <c r="C33" s="5"/>
-      <c r="D33" s="5"/>
-      <c r="E33" s="5"/>
-      <c r="F33" s="5"/>
+      <c r="B33" s="18"/>
+      <c r="C33" s="18"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="18"/>
     </row>
     <row r="34" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B34" s="5"/>
-      <c r="C34" s="5"/>
-      <c r="D34" s="5"/>
-      <c r="E34" s="5"/>
-      <c r="F34" s="5"/>
+      <c r="B34" s="18"/>
+      <c r="C34" s="18"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="18"/>
     </row>
     <row r="35" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B35" s="5"/>
-      <c r="C35" s="5"/>
-      <c r="D35" s="5"/>
-      <c r="E35" s="5"/>
-      <c r="F35" s="5"/>
+      <c r="B35" s="18"/>
+      <c r="C35" s="18"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="18"/>
+      <c r="F35" s="18"/>
     </row>
     <row r="36" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B36" s="5"/>
-      <c r="C36" s="5"/>
-      <c r="D36" s="5"/>
-      <c r="E36" s="5"/>
-      <c r="F36" s="5"/>
+      <c r="B36" s="18"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="18"/>
+      <c r="F36" s="18"/>
     </row>
     <row r="37" spans="2:6" ht="15.75" customHeight="1"/>
     <row r="38" spans="2:6" ht="15.75" customHeight="1"/>
@@ -4777,7 +5152,7 @@
   <dimension ref="A1:K1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -4831,18 +5206,18 @@
         <f t="shared" ref="C2:C12" si="1">TAN(RADIANS(B2))</f>
         <v>0.30573068145866039</v>
       </c>
-      <c r="D2" s="17">
+      <c r="D2" s="13">
         <f t="shared" ref="D2:D12" si="2">C2*$K$2</f>
         <v>402.02895567989827</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
-      <c r="F2" s="17">
+      <c r="F2" s="13">
         <f t="shared" ref="F2:F12" si="3">D2-E2</f>
         <v>402.02895567989827</v>
       </c>
-      <c r="G2" s="6">
+      <c r="G2" s="5">
         <f>(F2-$D$2)/$D$2</f>
         <v>0</v>
       </c>
@@ -4869,18 +5244,18 @@
         <f t="shared" si="1"/>
         <v>0.36397023426620234</v>
       </c>
-      <c r="D3" s="17">
+      <c r="D3" s="13">
         <f t="shared" si="2"/>
         <v>478.61265504160701</v>
       </c>
       <c r="E3">
         <v>77</v>
       </c>
-      <c r="F3" s="17">
+      <c r="F3" s="13">
         <f t="shared" si="3"/>
         <v>401.61265504160701</v>
       </c>
-      <c r="G3" s="6">
+      <c r="G3" s="5">
         <f t="shared" ref="G3:G12" si="4">(F3-$D$2)/$D$2</f>
         <v>-1.0354991410686507E-3</v>
       </c>
@@ -4897,18 +5272,18 @@
         <f t="shared" si="1"/>
         <v>0.41421356237309503</v>
       </c>
-      <c r="D4" s="17">
+      <c r="D4" s="13">
         <f t="shared" si="2"/>
         <v>544.68149913773937</v>
       </c>
       <c r="E4">
         <v>141</v>
       </c>
-      <c r="F4" s="17">
+      <c r="F4" s="13">
         <f t="shared" si="3"/>
         <v>403.68149913773937</v>
       </c>
-      <c r="G4" s="6">
+      <c r="G4" s="5">
         <f t="shared" si="4"/>
         <v>4.1105085454513175E-3</v>
       </c>
@@ -4925,18 +5300,18 @@
         <f t="shared" si="1"/>
         <v>0.46630765815499858</v>
       </c>
-      <c r="D5" s="17">
+      <c r="D5" s="13">
         <f t="shared" si="2"/>
         <v>613.18406101463484</v>
       </c>
       <c r="E5">
         <v>209</v>
       </c>
-      <c r="F5" s="17">
+      <c r="F5" s="13">
         <f t="shared" si="3"/>
         <v>404.18406101463484</v>
       </c>
-      <c r="G5" s="6">
+      <c r="G5" s="5">
         <f t="shared" si="4"/>
         <v>5.3605724271574345E-3</v>
       </c>
@@ -4953,18 +5328,18 @@
         <f t="shared" si="1"/>
         <v>0.52056705055174624</v>
       </c>
-      <c r="D6" s="17">
+      <c r="D6" s="13">
         <f t="shared" si="2"/>
         <v>684.53393913944399</v>
       </c>
       <c r="E6">
         <v>278</v>
       </c>
-      <c r="F6" s="17">
+      <c r="F6" s="13">
         <f t="shared" si="3"/>
         <v>406.53393913944399</v>
       </c>
-      <c r="G6" s="6">
+      <c r="G6" s="5">
         <f t="shared" si="4"/>
         <v>1.1205619386113698E-2</v>
       </c>
@@ -4981,18 +5356,18 @@
         <f t="shared" si="1"/>
         <v>0.57735026918962573</v>
       </c>
-      <c r="D7" s="17">
+      <c r="D7" s="13">
         <f t="shared" si="2"/>
         <v>759.20259189033516</v>
       </c>
       <c r="E7">
         <v>351</v>
       </c>
-      <c r="F7" s="17">
+      <c r="F7" s="13">
         <f t="shared" si="3"/>
         <v>408.20259189033516</v>
       </c>
-      <c r="G7" s="6">
+      <c r="G7" s="5">
         <f t="shared" si="4"/>
         <v>1.5356197913645871E-2</v>
       </c>
@@ -5009,18 +5384,18 @@
         <f t="shared" si="1"/>
         <v>0.63707026080749318</v>
       </c>
-      <c r="D8" s="17">
+      <c r="D8" s="13">
         <f t="shared" si="2"/>
         <v>837.73303492207231</v>
       </c>
       <c r="E8">
         <v>427</v>
       </c>
-      <c r="F8" s="17">
+      <c r="F8" s="13">
         <f t="shared" si="3"/>
         <v>410.73303492207231</v>
       </c>
-      <c r="G8" s="6">
+      <c r="G8" s="5">
         <f t="shared" si="4"/>
         <v>2.1650378957042974E-2</v>
       </c>
@@ -5037,18 +5412,18 @@
         <f t="shared" si="1"/>
         <v>0.70020753820970971</v>
       </c>
-      <c r="D9" s="17">
+      <c r="D9" s="13">
         <f t="shared" si="2"/>
         <v>920.75713174278133</v>
       </c>
       <c r="E9">
         <v>510</v>
       </c>
-      <c r="F9" s="17">
+      <c r="F9" s="13">
         <f t="shared" si="3"/>
         <v>410.75713174278133</v>
       </c>
-      <c r="G9" s="6">
+      <c r="G9" s="5">
         <f t="shared" si="4"/>
         <v>2.1710316979836053E-2</v>
       </c>
@@ -5065,18 +5440,18 @@
         <f t="shared" si="1"/>
         <v>0.76732698797896037</v>
       </c>
-      <c r="D10" s="17">
+      <c r="D10" s="13">
         <f t="shared" si="2"/>
         <v>1009.0176954775005</v>
       </c>
       <c r="E10">
         <v>593</v>
       </c>
-      <c r="F10" s="17">
+      <c r="F10" s="13">
         <f t="shared" si="3"/>
         <v>416.01769547750052</v>
       </c>
-      <c r="G10" s="6">
+      <c r="G10" s="5">
         <f t="shared" si="4"/>
         <v>3.4795353916597743E-2</v>
       </c>
@@ -5093,18 +5468,18 @@
         <f t="shared" si="1"/>
         <v>0.83909963117727993</v>
       </c>
-      <c r="D11" s="17">
+      <c r="D11" s="13">
         <f t="shared" si="2"/>
         <v>1103.3971036995961</v>
       </c>
       <c r="E11">
         <v>684</v>
       </c>
-      <c r="F11" s="17">
+      <c r="F11" s="13">
         <f t="shared" si="3"/>
         <v>419.39710369959607</v>
       </c>
-      <c r="G11" s="6">
+      <c r="G11" s="5">
         <f t="shared" si="4"/>
         <v>4.3201236563484222E-2</v>
       </c>
@@ -5121,148 +5496,148 @@
         <f t="shared" si="1"/>
         <v>0.90040404429783993</v>
       </c>
-      <c r="D12" s="17">
+      <c r="D12" s="13">
         <f t="shared" si="2"/>
         <v>1184.0110252983034</v>
       </c>
       <c r="E12">
         <v>760</v>
       </c>
-      <c r="F12" s="17">
+      <c r="F12" s="13">
         <f t="shared" si="3"/>
         <v>424.01102529830337</v>
       </c>
-      <c r="G12" s="6">
+      <c r="G12" s="5">
         <f t="shared" si="4"/>
         <v>5.4677826827746107E-2</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="15" customHeight="1">
-      <c r="B14" s="17">
+      <c r="B14" s="13">
         <f>D2-$D$2</f>
         <v>0</v>
       </c>
-      <c r="C14" s="17">
+      <c r="C14" s="13">
         <f>B14-E2</f>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="15" customHeight="1">
-      <c r="B15" s="17">
-        <f t="shared" ref="B15:B27" si="5">D3-$D$2</f>
+      <c r="B15" s="13">
+        <f t="shared" ref="B15:B24" si="5">D3-$D$2</f>
         <v>76.583699361708739</v>
       </c>
-      <c r="C15" s="17">
+      <c r="C15" s="13">
         <f t="shared" ref="C15:C24" si="6">B15-E3</f>
         <v>-0.41630063829126129</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="15" customHeight="1">
-      <c r="B16" s="17">
+      <c r="B16" s="13">
         <f t="shared" si="5"/>
         <v>142.65254345784109</v>
       </c>
-      <c r="C16" s="17">
+      <c r="C16" s="13">
         <f t="shared" si="6"/>
         <v>1.6525434578410909</v>
       </c>
     </row>
     <row r="17" spans="2:6" ht="15" customHeight="1">
-      <c r="B17" s="17">
+      <c r="B17" s="13">
         <f t="shared" si="5"/>
         <v>211.15510533473656</v>
       </c>
-      <c r="C17" s="17">
+      <c r="C17" s="13">
         <f t="shared" si="6"/>
         <v>2.155105334736561</v>
       </c>
     </row>
     <row r="18" spans="2:6" ht="15" customHeight="1">
-      <c r="B18" s="17">
+      <c r="B18" s="13">
         <f t="shared" si="5"/>
         <v>282.50498345954571</v>
       </c>
-      <c r="C18" s="17">
+      <c r="C18" s="13">
         <f t="shared" si="6"/>
         <v>4.5049834595457128</v>
       </c>
     </row>
     <row r="19" spans="2:6" ht="15" customHeight="1">
-      <c r="B19" s="17">
+      <c r="B19" s="13">
         <f t="shared" si="5"/>
         <v>357.17363621043688</v>
       </c>
-      <c r="C19" s="17">
+      <c r="C19" s="13">
         <f t="shared" si="6"/>
         <v>6.1736362104368823</v>
       </c>
     </row>
     <row r="20" spans="2:6" ht="15" customHeight="1">
-      <c r="B20" s="17">
+      <c r="B20" s="13">
         <f t="shared" si="5"/>
         <v>435.70407924217403</v>
       </c>
-      <c r="C20" s="17">
+      <c r="C20" s="13">
         <f t="shared" si="6"/>
         <v>8.7040792421740321</v>
       </c>
     </row>
     <row r="21" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B21" s="17">
+      <c r="B21" s="13">
         <f t="shared" si="5"/>
         <v>518.72817606288299</v>
       </c>
-      <c r="C21" s="17">
+      <c r="C21" s="13">
         <f t="shared" si="6"/>
         <v>8.7281760628829943</v>
       </c>
     </row>
     <row r="22" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B22" s="17">
+      <c r="B22" s="13">
         <f t="shared" si="5"/>
         <v>606.98873979760219</v>
       </c>
-      <c r="C22" s="17">
+      <c r="C22" s="13">
         <f t="shared" si="6"/>
         <v>13.988739797602193</v>
       </c>
     </row>
     <row r="23" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B23" s="17">
+      <c r="B23" s="13">
         <f t="shared" si="5"/>
         <v>701.36814801969786</v>
       </c>
-      <c r="C23" s="17">
+      <c r="C23" s="13">
         <f t="shared" si="6"/>
         <v>17.368148019697855</v>
       </c>
     </row>
     <row r="24" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B24" s="17">
+      <c r="B24" s="13">
         <f t="shared" si="5"/>
         <v>781.98206961840515</v>
       </c>
-      <c r="C24" s="17">
+      <c r="C24" s="13">
         <f t="shared" si="6"/>
         <v>21.982069618405149</v>
       </c>
     </row>
     <row r="25" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B25" s="17"/>
+      <c r="B25" s="13"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
     </row>
     <row r="26" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B26" s="17"/>
+      <c r="B26" s="13"/>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
     </row>
     <row r="27" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B27" s="17"/>
+      <c r="B27" s="13"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
@@ -6294,7 +6669,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -6303,7 +6680,8 @@
     <col min="4" max="4" width="15.140625" customWidth="1"/>
     <col min="5" max="5" width="21.85546875" customWidth="1"/>
     <col min="6" max="6" width="19" customWidth="1"/>
-    <col min="7" max="9" width="8.7109375" customWidth="1"/>
+    <col min="7" max="8" width="8.7109375" customWidth="1"/>
+    <col min="9" max="9" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="23.85546875" customWidth="1"/>
     <col min="11" max="26" width="8.7109375" customWidth="1"/>
   </cols>
@@ -6396,7 +6774,7 @@
         <v>401.61265504160701</v>
       </c>
       <c r="G3">
-        <f t="shared" si="4"/>
+        <f>F3/$D$2</f>
         <v>0.9989645008589314</v>
       </c>
     </row>
@@ -6657,76 +7035,76 @@
     <row r="23" spans="2:6" ht="15.75" customHeight="1"/>
     <row r="24" spans="2:6" ht="15.75" customHeight="1"/>
     <row r="25" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B25" s="4" t="s">
+      <c r="B25" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="5"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
     </row>
     <row r="26" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B26" s="5"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="5"/>
+      <c r="B26" s="18"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
     </row>
     <row r="27" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B27" s="5"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="5"/>
-      <c r="F27" s="5"/>
+      <c r="B27" s="18"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
     </row>
     <row r="28" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B28" s="5"/>
-      <c r="C28" s="5"/>
-      <c r="D28" s="5"/>
-      <c r="E28" s="5"/>
-      <c r="F28" s="5"/>
+      <c r="B28" s="18"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
     </row>
     <row r="29" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B29" s="5"/>
-      <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="5"/>
-      <c r="F29" s="5"/>
+      <c r="B29" s="18"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="18"/>
     </row>
     <row r="30" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B30" s="5"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="5"/>
-      <c r="E30" s="5"/>
-      <c r="F30" s="5"/>
+      <c r="B30" s="18"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="18"/>
     </row>
     <row r="31" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B31" s="5"/>
-      <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
-      <c r="E31" s="5"/>
-      <c r="F31" s="5"/>
+      <c r="B31" s="18"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="18"/>
     </row>
     <row r="32" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B32" s="5"/>
-      <c r="C32" s="5"/>
-      <c r="D32" s="5"/>
-      <c r="E32" s="5"/>
-      <c r="F32" s="5"/>
+      <c r="B32" s="18"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="18"/>
     </row>
     <row r="33" spans="2:7" ht="15.75" customHeight="1">
-      <c r="B33" s="5"/>
-      <c r="C33" s="5"/>
-      <c r="D33" s="5"/>
-      <c r="E33" s="5"/>
-      <c r="F33" s="5"/>
+      <c r="B33" s="18"/>
+      <c r="C33" s="18"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="18"/>
     </row>
     <row r="34" spans="2:7" ht="15.75" customHeight="1">
-      <c r="B34" s="5"/>
-      <c r="C34" s="5"/>
-      <c r="D34" s="5"/>
-      <c r="E34" s="5"/>
-      <c r="F34" s="5"/>
+      <c r="B34" s="18"/>
+      <c r="C34" s="18"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="18"/>
     </row>
     <row r="35" spans="2:7" ht="15.75" customHeight="1"/>
     <row r="36" spans="2:7" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
word crashed and lost work so I'm backing it up to make sure I don't lose more
</commit_message>
<xml_diff>
--- a/Testing/Relative Positioning/Altitude Relative Measure/Altitude Relative Measure Calculations.xlsx
+++ b/Testing/Relative Positioning/Altitude Relative Measure/Altitude Relative Measure Calculations.xlsx
@@ -9,18 +9,19 @@
   <sheets>
     <sheet name="Az=0 (4-3-18)" sheetId="1" r:id="rId1"/>
     <sheet name="Az=0 Plot with Error bars" sheetId="6" r:id="rId2"/>
-    <sheet name="Az=0 cmd vs cmd-calc" sheetId="7" r:id="rId3"/>
-    <sheet name="Az=0 (4-4-18 retest)" sheetId="2" r:id="rId4"/>
-    <sheet name="Az=10 (4-4-18)" sheetId="3" r:id="rId5"/>
-    <sheet name="Az=10 (4-6-18)(angle apparatus)" sheetId="4" r:id="rId6"/>
-    <sheet name="Grid Measurements" sheetId="5" r:id="rId7"/>
+    <sheet name="Az=10 cmd vs cmd-calc" sheetId="8" r:id="rId3"/>
+    <sheet name="Az=0 cmd vs cmd-calc" sheetId="7" r:id="rId4"/>
+    <sheet name="Az=0 (4-4-18 retest)" sheetId="2" r:id="rId5"/>
+    <sheet name="Az=10 (4-4-18)" sheetId="3" r:id="rId6"/>
+    <sheet name="Az=10 (4-6-18)(angle apparatus)" sheetId="4" r:id="rId7"/>
+    <sheet name="Grid Measurements" sheetId="5" r:id="rId8"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="37">
   <si>
     <t>TAN</t>
   </si>
@@ -150,13 +151,16 @@
     <t>Calculated Angle</t>
   </si>
   <si>
-    <t>Cmd minus Calc Angle</t>
+    <t>Cmd Angle - Calc Angle</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="169" formatCode="0.0000"/>
+  </numFmts>
   <fonts count="5">
     <font>
       <sz val="11"/>
@@ -335,11 +339,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -353,6 +356,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -366,6 +370,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -468,11 +473,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="133976448"/>
-        <c:axId val="133985408"/>
+        <c:axId val="65345024"/>
+        <c:axId val="65346944"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="133976448"/>
+        <c:axId val="65345024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -506,12 +511,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="133985408"/>
+        <c:crossAx val="65346944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="133985408"/>
+        <c:axId val="65346944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -545,7 +550,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="133976448"/>
+        <c:crossAx val="65345024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -787,11 +792,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="165119488"/>
-        <c:axId val="165121408"/>
+        <c:axId val="65536000"/>
+        <c:axId val="65537920"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="165119488"/>
+        <c:axId val="65536000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -813,18 +818,19 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="165121408"/>
+        <c:crossAx val="65537920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="165121408"/>
+        <c:axId val="65537920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -852,13 +858,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="165119488"/>
+        <c:crossAx val="65536000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -900,10 +907,10 @@
           </c:spPr>
           <c:xVal>
             <c:numRef>
-              <c:f>'Az=0 (4-4-18 retest)'!$B$3:$B$14</c:f>
+              <c:f>'Az=10 (4-4-18)'!$B$2:$B$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>17</c:v>
                 </c:pt>
@@ -936,54 +943,48 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>42</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>45</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Az=0 (4-4-18 retest)'!$I$3:$I$14</c:f>
+              <c:f>'Az=10 (4-4-18)'!$I$2:$I$12</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>-4.9868769295358106E-5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.2599586120112036E-2</c:v>
+                  <c:v>6.1646955805755965E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-1.8377251557794239E-2</c:v>
+                  <c:v>1.9386954775139742E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-0.10724365958140325</c:v>
+                  <c:v>3.820433061657269E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-7.7136005254676121E-2</c:v>
+                  <c:v>-7.4614641266492754E-3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-5.8057469727032185E-2</c:v>
+                  <c:v>-2.4846878330158972E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-0.19194047953175186</c:v>
+                  <c:v>-6.5696152403099006E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-0.20383212795654515</c:v>
+                  <c:v>-2.5205861868293766E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-0.32916294883163744</c:v>
+                  <c:v>-0.13302571336235047</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-0.38416899017933304</c:v>
+                  <c:v>-0.17476415609235829</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-0.51984098395346479</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>-0.58278822910520489</c:v>
+                  <c:v>-0.24782536131517929</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -998,11 +999,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="165141888"/>
-        <c:axId val="165156352"/>
+        <c:axId val="76447744"/>
+        <c:axId val="76449664"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="165141888"/>
+        <c:axId val="76447744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="46"/>
@@ -1038,12 +1039,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="165156352"/>
+        <c:crossAx val="76449664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="165156352"/>
+        <c:axId val="76449664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="5.000000000000001E-2"/>
@@ -1076,11 +1077,11 @@
           <c:layout/>
           <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.0000" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="165141888"/>
+        <c:crossAx val="76447744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1093,6 +1094,228 @@
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Az=0 (4-4-18 retest)'!$B$3:$B$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>22.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>27.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>32.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>37.5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>45</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Az=0 (4-4-18 retest)'!$I$3:$I$14</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>-4.9868769295358106E-5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.2599586120112036E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-1.8377251557794239E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-0.10724365958140325</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-7.7136005254676121E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-5.8057469727032185E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-0.19194047953175186</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-0.20383212795654515</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-0.32916294883163744</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-0.38416899017933304</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-0.51984098395346479</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-0.58278822910520489</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="65615744"/>
+        <c:axId val="65622016"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="65615744"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="46"/>
+          <c:min val="15"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Command</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Angle [deg]</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="65622016"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="65622016"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="5.000000000000001E-2"/>
+          <c:min val="-0.60000000000000009"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Command Angle minus</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Calculated Angle [deg]</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="0.0000" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="65615744"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1227,11 +1450,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="165303424"/>
-        <c:axId val="165305344"/>
+        <c:axId val="100994432"/>
+        <c:axId val="101008896"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="165303424"/>
+        <c:axId val="100994432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1265,12 +1488,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="165305344"/>
+        <c:crossAx val="101008896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="165305344"/>
+        <c:axId val="101008896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1304,7 +1527,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="165303424"/>
+        <c:crossAx val="100994432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1316,253 +1539,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="zero"/>
-    <c:showDLblsOverMax val="1"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="1"/>
-  <c:style val="2"/>
-  <c:chart>
-    <c:autoTitleDeleted val="1"/>
-    <c:plotArea>
       <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:ln w="47625">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="7"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="4F81BD"/>
-              </a:solidFill>
-              <a:ln cmpd="sng">
-                <a:solidFill>
-                  <a:srgbClr val="4F81BD"/>
-                </a:solidFill>
-              </a:ln>
-            </c:spPr>
-          </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-              </a:ln>
-            </c:spPr>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="1"/>
-            <c:dispEq val="0"/>
-            <c:trendlineLbl>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-            </c:trendlineLbl>
-          </c:trendline>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'Az=10 (4-4-18)'!$D$2:$D$12</c:f>
-              <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>402.02895567989827</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>478.61265504160701</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>544.68149913773937</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>613.18406101463484</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>684.53393913944399</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>759.20259189033516</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>837.73303492207231</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>920.75713174278133</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1009.0176954775005</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1103.3971036995961</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1184.0110252983034</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'Az=10 (4-4-18)'!$G$2:$G$12</c:f>
-              <c:numCache>
-                <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>-1.0354991410686507E-3</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4.1105085454513175E-3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5.3605724271574345E-3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.1205619386113698E-2</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.5356197913645871E-2</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2.1650378957042974E-2</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2.1710316979836053E-2</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>3.4795353916597743E-2</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>4.3201236563484222E-2</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>5.4677826827746107E-2</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="165350784"/>
-        <c:axId val="165364864"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="165350784"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
-        <c:majorTickMark val="cross"/>
-        <c:minorTickMark val="cross"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="47625">
-            <a:noFill/>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr lvl="0">
-              <a:defRPr b="0"/>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="165364864"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="165364864"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:srgbClr val="B7B7B7"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
-        <c:majorTickMark val="cross"/>
-        <c:minorTickMark val="cross"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="47625">
-            <a:noFill/>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr lvl="0">
-              <a:defRPr b="0"/>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="165350784"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:solidFill>
-          <a:srgbClr val="FFFFFF"/>
-        </a:solidFill>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1624,14 +1601,15 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="0"/>
             <c:trendlineLbl>
+              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Az=10 (4-6-18)(angle apparatus)'!$D$2:$D$12</c:f>
+              <c:f>'Az=10 (4-4-18)'!$D$2:$D$12</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>402.02895567989827</c:v>
@@ -1671,42 +1649,42 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Az=10 (4-6-18)(angle apparatus)'!$G$2:$G$12</c:f>
+              <c:f>'Az=10 (4-4-18)'!$G$2:$G$12</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.9989645008589314</c:v>
+                  <c:v>-1.0354991410686507E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.0041105085454514</c:v>
+                  <c:v>4.1105085454513175E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.0053605724271575</c:v>
+                  <c:v>5.3605724271574345E-3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.0112056193861136</c:v>
+                  <c:v>1.1205619386113698E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.0153561979136458</c:v>
+                  <c:v>1.5356197913645871E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.021650378957043</c:v>
+                  <c:v>2.1650378957042974E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.0217103169798361</c:v>
+                  <c:v>2.1710316979836053E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.0347953539165977</c:v>
+                  <c:v>3.4795353916597743E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.0432012365634842</c:v>
+                  <c:v>4.3201236563484222E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.0546778268277461</c:v>
+                  <c:v>5.4677826827746107E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1721,11 +1699,260 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="165402880"/>
-        <c:axId val="165404672"/>
+        <c:axId val="101043584"/>
+        <c:axId val="101049472"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="165402880"/>
+        <c:axId val="101043584"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="cross"/>
+        <c:minorTickMark val="cross"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="47625">
+            <a:noFill/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="101049472"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="101049472"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="B7B7B7"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+        <c:majorTickMark val="cross"/>
+        <c:minorTickMark val="cross"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="47625">
+            <a:noFill/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="101043584"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="1"/>
+  <c:style val="2"/>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="47625">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="7"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="4F81BD"/>
+              </a:solidFill>
+              <a:ln cmpd="sng">
+                <a:solidFill>
+                  <a:srgbClr val="4F81BD"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="0"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Az=10 (4-6-18)(angle apparatus)'!$D$2:$D$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>402.02895567989827</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>478.61265504160701</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>544.68149913773937</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>613.18406101463484</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>684.53393913944399</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>759.20259189033516</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>837.73303492207231</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>920.75713174278133</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1009.0176954775005</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1103.3971036995961</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1184.0110252983034</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Az=10 (4-6-18)(angle apparatus)'!$G$2:$G$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.9989645008589314</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0041105085454514</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0053605724271575</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.0112056193861136</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.0153561979136458</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.021650378957043</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.0217103169798361</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.0347953539165977</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.0432012365634842</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.0546778268277461</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="122108160"/>
+        <c:axId val="122126336"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="122108160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1759,12 +1986,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="165404672"/>
+        <c:crossAx val="122126336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="165404672"/>
+        <c:axId val="122126336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1798,7 +2025,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="165402880"/>
+        <c:crossAx val="122108160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1810,6 +2037,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1840,6 +2068,17 @@
   <sheetPr/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="125" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1880,7 +2119,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8671034" cy="6293069"/>
+    <xdr:ext cx="8663609" cy="6286500"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -1932,6 +2171,33 @@
 
 <file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8671560" cy="6294120"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
@@ -1960,11 +2226,11 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>590550</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
@@ -1990,7 +2256,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
@@ -3457,7 +3723,7 @@
   <dimension ref="A1:T1001"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="H2" sqref="H2:I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -3470,7 +3736,8 @@
     <col min="6" max="6" width="27.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.7109375" customWidth="1"/>
     <col min="8" max="8" width="16" bestFit="1" customWidth="1"/>
-    <col min="9" max="26" width="8.7109375" customWidth="1"/>
+    <col min="9" max="9" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" s="3" customFormat="1" ht="15" customHeight="1">
@@ -3484,38 +3751,38 @@
       <c r="G1" s="21"/>
     </row>
     <row r="2" spans="1:20">
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="H2" s="15" t="s">
+      <c r="H2" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="I2" s="16" t="s">
+      <c r="I2" s="15" t="s">
         <v>36</v>
       </c>
       <c r="K2" t="s">
         <v>9</v>
       </c>
-      <c r="S2" s="13">
+      <c r="S2" s="12">
         <f>D3-$D$3</f>
         <v>0</v>
       </c>
-      <c r="T2" s="13">
+      <c r="T2" s="12">
         <f>S2-E3</f>
         <v>0</v>
       </c>
@@ -3525,44 +3792,44 @@
         <f t="shared" ref="A3:A14" si="0">RADIANS(B3)</f>
         <v>0.29670597283903605</v>
       </c>
-      <c r="B3" s="7">
+      <c r="B3" s="6">
         <v>17</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="5">
         <f t="shared" ref="C3:C14" si="1">TAN(RADIANS(B3))</f>
         <v>0.30573068145866039</v>
       </c>
-      <c r="D3" s="11">
+      <c r="D3" s="10">
         <f t="shared" ref="D3:D14" si="2">C3*$K$3</f>
         <v>395.92123248896519</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3" s="5">
         <v>0</v>
       </c>
-      <c r="F3" s="11">
+      <c r="F3" s="10">
         <f t="shared" ref="F3:F14" si="3">D3-E3</f>
         <v>395.92123248896519</v>
       </c>
-      <c r="G3" s="14">
+      <c r="G3" s="13">
         <f>(F3-$D$3)/$D$3*100</f>
         <v>0</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="22">
         <f>DEGREES(ATAN((E3+395.92)/1295))</f>
         <v>16.999950131230705</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="22">
         <f>H3-B3</f>
         <v>-4.9868769295358106E-5</v>
       </c>
       <c r="K3">
         <v>1295</v>
       </c>
-      <c r="S3" s="13">
+      <c r="S3" s="12">
         <f t="shared" ref="S3:S12" si="4">D4-$D$3</f>
         <v>75.420220885766867</v>
       </c>
-      <c r="T3" s="13">
+      <c r="T3" s="12">
         <f>S3-E4</f>
         <v>-0.57977911423313344</v>
       </c>
@@ -3572,41 +3839,41 @@
         <f t="shared" si="0"/>
         <v>0.3490658503988659</v>
       </c>
-      <c r="B4" s="7">
+      <c r="B4" s="6">
         <v>20</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="5">
         <f t="shared" si="1"/>
         <v>0.36397023426620234</v>
       </c>
-      <c r="D4" s="11">
+      <c r="D4" s="10">
         <f t="shared" si="2"/>
         <v>471.34145337473205</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="5">
         <v>76</v>
       </c>
-      <c r="F4" s="11">
+      <c r="F4" s="10">
         <f t="shared" si="3"/>
         <v>395.34145337473205</v>
       </c>
-      <c r="G4" s="14">
+      <c r="G4" s="13">
         <f t="shared" ref="G4:G14" si="5">(F4-$D$3)/$D$3*100</f>
         <v>-0.14643799489821313</v>
       </c>
-      <c r="H4" s="4">
+      <c r="H4" s="22">
         <f t="shared" ref="H4:H14" si="6">DEGREES(ATAN((E4+395.92)/1295))</f>
         <v>20.022599586120112</v>
       </c>
-      <c r="I4" s="4">
+      <c r="I4" s="22">
         <f t="shared" ref="I4:I14" si="7">H4-B4</f>
         <v>2.2599586120112036E-2</v>
       </c>
-      <c r="S4" s="13">
+      <c r="S4" s="12">
         <f t="shared" si="4"/>
         <v>140.48533078419291</v>
       </c>
-      <c r="T4" s="13">
+      <c r="T4" s="12">
         <f t="shared" ref="T4:T13" si="8">S4-E5</f>
         <v>0.48533078419291087</v>
       </c>
@@ -3616,41 +3883,41 @@
         <f t="shared" si="0"/>
         <v>0.39269908169872414</v>
       </c>
-      <c r="B5" s="7">
+      <c r="B5" s="6">
         <v>22.5</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="5">
         <f t="shared" si="1"/>
         <v>0.41421356237309503</v>
       </c>
-      <c r="D5" s="11">
+      <c r="D5" s="10">
         <f t="shared" si="2"/>
         <v>536.4065632731581</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="5">
         <v>140</v>
       </c>
-      <c r="F5" s="11">
+      <c r="F5" s="10">
         <f t="shared" si="3"/>
         <v>396.4065632731581</v>
       </c>
-      <c r="G5" s="14">
+      <c r="G5" s="13">
         <f t="shared" si="5"/>
         <v>0.12258266149099181</v>
       </c>
-      <c r="H5" s="4">
+      <c r="H5" s="22">
         <f t="shared" si="6"/>
         <v>22.481622748442206</v>
       </c>
-      <c r="I5" s="4">
+      <c r="I5" s="22">
         <f t="shared" si="7"/>
         <v>-1.8377251557794239E-2</v>
       </c>
-      <c r="S5" s="13">
+      <c r="S5" s="12">
         <f t="shared" si="4"/>
         <v>207.94718482175801</v>
       </c>
-      <c r="T5" s="13">
+      <c r="T5" s="12">
         <f t="shared" si="8"/>
         <v>2.9471848217580146</v>
       </c>
@@ -3660,41 +3927,41 @@
         <f t="shared" si="0"/>
         <v>0.43633231299858238</v>
       </c>
-      <c r="B6" s="7">
+      <c r="B6" s="6">
         <v>25</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="5">
         <f t="shared" si="1"/>
         <v>0.46630765815499858</v>
       </c>
-      <c r="D6" s="11">
+      <c r="D6" s="10">
         <f t="shared" si="2"/>
         <v>603.8684173107232</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="5">
         <v>205</v>
       </c>
-      <c r="F6" s="11">
+      <c r="F6" s="10">
         <f t="shared" si="3"/>
         <v>398.8684173107232</v>
       </c>
-      <c r="G6" s="14">
+      <c r="G6" s="13">
         <f t="shared" si="5"/>
         <v>0.74438665570686613</v>
       </c>
-      <c r="H6" s="4">
+      <c r="H6" s="22">
         <f t="shared" si="6"/>
         <v>24.892756340418597</v>
       </c>
-      <c r="I6" s="4">
+      <c r="I6" s="22">
         <f t="shared" si="7"/>
         <v>-0.10724365958140325</v>
       </c>
-      <c r="S6" s="13">
+      <c r="S6" s="12">
         <f t="shared" si="4"/>
         <v>278.21309797554613</v>
       </c>
-      <c r="T6" s="13">
+      <c r="T6" s="12">
         <f t="shared" si="8"/>
         <v>2.213097975546134</v>
       </c>
@@ -3704,41 +3971,41 @@
         <f t="shared" si="0"/>
         <v>0.47996554429844063</v>
       </c>
-      <c r="B7" s="7">
+      <c r="B7" s="6">
         <v>27.5</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="5">
         <f t="shared" si="1"/>
         <v>0.52056705055174624</v>
       </c>
-      <c r="D7" s="11">
+      <c r="D7" s="10">
         <f t="shared" si="2"/>
         <v>674.13433046451132</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="5">
         <v>276</v>
       </c>
-      <c r="F7" s="11">
+      <c r="F7" s="10">
         <f t="shared" si="3"/>
         <v>398.13433046451132</v>
       </c>
-      <c r="G7" s="14">
+      <c r="G7" s="13">
         <f t="shared" si="5"/>
         <v>0.55897430951946125</v>
       </c>
-      <c r="H7" s="4">
+      <c r="H7" s="22">
         <f t="shared" si="6"/>
         <v>27.422863994745324</v>
       </c>
-      <c r="I7" s="4">
+      <c r="I7" s="22">
         <f t="shared" si="7"/>
         <v>-7.7136005254676121E-2</v>
       </c>
-      <c r="S7" s="13">
+      <c r="S7" s="12">
         <f t="shared" si="4"/>
         <v>351.74736611160017</v>
       </c>
-      <c r="T7" s="13">
+      <c r="T7" s="12">
         <f t="shared" si="8"/>
         <v>1.7473661116001722</v>
       </c>
@@ -3748,41 +4015,41 @@
         <f t="shared" si="0"/>
         <v>0.52359877559829882</v>
       </c>
-      <c r="B8" s="7">
+      <c r="B8" s="6">
         <v>30</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="5">
         <f t="shared" si="1"/>
         <v>0.57735026918962573</v>
       </c>
-      <c r="D8" s="11">
+      <c r="D8" s="10">
         <f t="shared" si="2"/>
         <v>747.66859860056536</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="5">
         <v>350</v>
       </c>
-      <c r="F8" s="11">
+      <c r="F8" s="10">
         <f t="shared" si="3"/>
         <v>397.66859860056536</v>
       </c>
-      <c r="G8" s="14">
+      <c r="G8" s="13">
         <f t="shared" si="5"/>
         <v>0.44134185494809841</v>
       </c>
-      <c r="H8" s="4">
+      <c r="H8" s="22">
         <f t="shared" si="6"/>
         <v>29.941942530272968</v>
       </c>
-      <c r="I8" s="4">
+      <c r="I8" s="22">
         <f t="shared" si="7"/>
         <v>-5.8057469727032185E-2</v>
       </c>
-      <c r="S8" s="13">
+      <c r="S8" s="12">
         <f t="shared" si="4"/>
         <v>429.0847552567385</v>
       </c>
-      <c r="T8" s="13">
+      <c r="T8" s="12">
         <f t="shared" si="8"/>
         <v>6.0847552567385037</v>
       </c>
@@ -3792,41 +4059,41 @@
         <f t="shared" si="0"/>
         <v>0.56723200689815712</v>
       </c>
-      <c r="B9" s="7">
+      <c r="B9" s="6">
         <v>32.5</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="5">
         <f t="shared" si="1"/>
         <v>0.63707026080749318</v>
       </c>
-      <c r="D9" s="11">
+      <c r="D9" s="10">
         <f t="shared" si="2"/>
         <v>825.00598774570369</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E9" s="5">
         <v>423</v>
       </c>
-      <c r="F9" s="11">
+      <c r="F9" s="10">
         <f>D9-E9</f>
         <v>402.00598774570369</v>
       </c>
-      <c r="G9" s="14">
+      <c r="G9" s="13">
         <f t="shared" si="5"/>
         <v>1.5368600513002528</v>
       </c>
-      <c r="H9" s="4">
+      <c r="H9" s="22">
         <f t="shared" si="6"/>
         <v>32.308059520468248</v>
       </c>
-      <c r="I9" s="4">
+      <c r="I9" s="22">
         <f t="shared" si="7"/>
         <v>-0.19194047953175186</v>
       </c>
-      <c r="S9" s="13">
+      <c r="S9" s="12">
         <f t="shared" si="4"/>
         <v>510.84752949260894</v>
       </c>
-      <c r="T9" s="13">
+      <c r="T9" s="12">
         <f t="shared" si="8"/>
         <v>6.8475294926089418</v>
       </c>
@@ -3836,41 +4103,41 @@
         <f t="shared" si="0"/>
         <v>0.6108652381980153</v>
       </c>
-      <c r="B10" s="7">
+      <c r="B10" s="6">
         <v>35</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="5">
         <f t="shared" si="1"/>
         <v>0.70020753820970971</v>
       </c>
-      <c r="D10" s="11">
+      <c r="D10" s="10">
         <f t="shared" si="2"/>
         <v>906.76876198157413</v>
       </c>
-      <c r="E10" s="6">
+      <c r="E10" s="5">
         <v>504</v>
       </c>
-      <c r="F10" s="11">
+      <c r="F10" s="10">
         <f t="shared" si="3"/>
         <v>402.76876198157413</v>
       </c>
-      <c r="G10" s="14">
+      <c r="G10" s="13">
         <f t="shared" si="5"/>
         <v>1.7295181290384043</v>
       </c>
-      <c r="H10" s="4">
+      <c r="H10" s="22">
         <f t="shared" si="6"/>
         <v>34.796167872043455</v>
       </c>
-      <c r="I10" s="4">
+      <c r="I10" s="22">
         <f t="shared" si="7"/>
         <v>-0.20383212795654515</v>
       </c>
-      <c r="S10" s="13">
+      <c r="S10" s="12">
         <f t="shared" si="4"/>
         <v>597.76721694378853</v>
       </c>
-      <c r="T10" s="13">
+      <c r="T10" s="12">
         <f t="shared" si="8"/>
         <v>11.767216943788526</v>
       </c>
@@ -3880,41 +4147,41 @@
         <f t="shared" si="0"/>
         <v>0.6544984694978736</v>
       </c>
-      <c r="B11" s="7">
+      <c r="B11" s="6">
         <v>37.5</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="5">
         <f t="shared" si="1"/>
         <v>0.76732698797896037</v>
       </c>
-      <c r="D11" s="11">
+      <c r="D11" s="10">
         <f t="shared" si="2"/>
         <v>993.68844943275371</v>
       </c>
-      <c r="E11" s="6">
+      <c r="E11" s="5">
         <v>586</v>
       </c>
-      <c r="F11" s="11">
+      <c r="F11" s="10">
         <f t="shared" si="3"/>
         <v>407.68844943275371</v>
       </c>
-      <c r="G11" s="14">
+      <c r="G11" s="13">
         <f t="shared" si="5"/>
         <v>2.9721106063985827</v>
       </c>
-      <c r="H11" s="4">
+      <c r="H11" s="22">
         <f t="shared" si="6"/>
         <v>37.170837051168363</v>
       </c>
-      <c r="I11" s="4">
+      <c r="I11" s="22">
         <f t="shared" si="7"/>
         <v>-0.32916294883163744</v>
       </c>
-      <c r="S11" s="13">
+      <c r="S11" s="12">
         <f t="shared" si="4"/>
         <v>690.71278988561221</v>
       </c>
-      <c r="T11" s="13">
+      <c r="T11" s="12">
         <f t="shared" si="8"/>
         <v>14.71278988561221</v>
       </c>
@@ -3924,41 +4191,41 @@
         <f t="shared" si="0"/>
         <v>0.69813170079773179</v>
       </c>
-      <c r="B12" s="7">
+      <c r="B12" s="6">
         <v>40</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12" s="5">
         <f t="shared" si="1"/>
         <v>0.83909963117727993</v>
       </c>
-      <c r="D12" s="11">
+      <c r="D12" s="10">
         <f t="shared" si="2"/>
         <v>1086.6340223745774</v>
       </c>
-      <c r="E12" s="6">
+      <c r="E12" s="5">
         <v>676</v>
       </c>
-      <c r="F12" s="11">
+      <c r="F12" s="10">
         <f t="shared" si="3"/>
         <v>410.6340223745774</v>
       </c>
-      <c r="G12" s="14">
+      <c r="G12" s="13">
         <f t="shared" si="5"/>
         <v>3.7160901407383533</v>
       </c>
-      <c r="H12" s="4">
+      <c r="H12" s="22">
         <f t="shared" si="6"/>
         <v>39.615831009820667</v>
       </c>
-      <c r="I12" s="4">
+      <c r="I12" s="22">
         <f t="shared" si="7"/>
         <v>-0.38416899017933304</v>
       </c>
-      <c r="S12" s="13">
+      <c r="S12" s="12">
         <f t="shared" si="4"/>
         <v>770.10200487673751</v>
       </c>
-      <c r="T12" s="13">
+      <c r="T12" s="12">
         <f t="shared" si="8"/>
         <v>21.10200487673751</v>
       </c>
@@ -3968,41 +4235,41 @@
         <f t="shared" si="0"/>
         <v>0.73303828583761843</v>
       </c>
-      <c r="B13" s="7">
+      <c r="B13" s="6">
         <v>42</v>
       </c>
-      <c r="C13" s="6">
+      <c r="C13" s="5">
         <f t="shared" si="1"/>
         <v>0.90040404429783993</v>
       </c>
-      <c r="D13" s="11">
+      <c r="D13" s="10">
         <f t="shared" si="2"/>
         <v>1166.0232373657027</v>
       </c>
-      <c r="E13" s="6">
+      <c r="E13" s="5">
         <v>749</v>
       </c>
-      <c r="F13" s="11">
+      <c r="F13" s="10">
         <f t="shared" si="3"/>
         <v>417.0232373657027</v>
       </c>
-      <c r="G13" s="14">
+      <c r="G13" s="13">
         <f t="shared" si="5"/>
         <v>5.3298492591769877</v>
       </c>
-      <c r="H13" s="4">
+      <c r="H13" s="22">
         <f t="shared" si="6"/>
         <v>41.480159016046535</v>
       </c>
-      <c r="I13" s="4">
+      <c r="I13" s="22">
         <f t="shared" si="7"/>
         <v>-0.51984098395346479</v>
       </c>
-      <c r="S13" s="13">
+      <c r="S13" s="12">
         <f>D14-$D$3</f>
         <v>899.07876751103458</v>
       </c>
-      <c r="T13" s="13">
+      <c r="T13" s="12">
         <f t="shared" si="8"/>
         <v>26.078767511034584</v>
       </c>
@@ -4012,37 +4279,37 @@
         <f t="shared" si="0"/>
         <v>0.78539816339744828</v>
       </c>
-      <c r="B14" s="9">
+      <c r="B14" s="8">
         <v>45</v>
       </c>
-      <c r="C14" s="10">
+      <c r="C14" s="9">
         <f t="shared" si="1"/>
         <v>0.99999999999999989</v>
       </c>
-      <c r="D14" s="12">
+      <c r="D14" s="11">
         <f t="shared" si="2"/>
         <v>1294.9999999999998</v>
       </c>
-      <c r="E14" s="10">
+      <c r="E14" s="9">
         <v>873</v>
       </c>
-      <c r="F14" s="12">
+      <c r="F14" s="11">
         <f t="shared" si="3"/>
         <v>421.99999999999977</v>
       </c>
-      <c r="G14" s="14">
+      <c r="G14" s="13">
         <f t="shared" si="5"/>
         <v>6.5868575289812048</v>
       </c>
-      <c r="H14" s="4">
+      <c r="H14" s="22">
         <f t="shared" si="6"/>
         <v>44.417211770894795</v>
       </c>
-      <c r="I14" s="4">
+      <c r="I14" s="22">
         <f t="shared" si="7"/>
         <v>-0.58278822910520489</v>
       </c>
-      <c r="S14" s="13"/>
+      <c r="S14" s="12"/>
     </row>
     <row r="17" spans="2:6">
       <c r="D17">
@@ -5149,10 +5416,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K1000"/>
+  <dimension ref="A1:L1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="H2" sqref="H2:I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -5162,13 +5429,15 @@
     <col min="4" max="4" width="15.140625" customWidth="1"/>
     <col min="5" max="5" width="21.85546875" customWidth="1"/>
     <col min="6" max="6" width="19" customWidth="1"/>
-    <col min="7" max="8" width="8.7109375" customWidth="1"/>
-    <col min="9" max="9" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="26" width="8.7109375" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.7109375" customWidth="1"/>
+    <col min="9" max="9" width="8.7109375" style="16" customWidth="1"/>
+    <col min="10" max="10" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="27" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:12">
       <c r="C1" t="s">
         <v>0</v>
       </c>
@@ -5184,17 +5453,23 @@
       <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="I1" t="s">
+      <c r="H1" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="I1" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1" t="s">
         <v>5</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>6</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:12">
       <c r="A2">
         <f t="shared" ref="A2:A12" si="0">RADIANS(B2)</f>
         <v>0.29670597283903605</v>
@@ -5206,33 +5481,41 @@
         <f t="shared" ref="C2:C12" si="1">TAN(RADIANS(B2))</f>
         <v>0.30573068145866039</v>
       </c>
-      <c r="D2" s="13">
-        <f t="shared" ref="D2:D12" si="2">C2*$K$2</f>
+      <c r="D2" s="12">
+        <f t="shared" ref="D2:D12" si="2">C2*$L$2</f>
         <v>402.02895567989827</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
-      <c r="F2" s="13">
+      <c r="F2" s="12">
         <f t="shared" ref="F2:F12" si="3">D2-E2</f>
         <v>402.02895567989827</v>
       </c>
-      <c r="G2" s="5">
+      <c r="G2" s="4">
         <f>(F2-$D$2)/$D$2</f>
         <v>0</v>
       </c>
-      <c r="I2">
+      <c r="H2" s="22">
+        <f>DEGREES(ATAN((E2+395.92)/1295))</f>
+        <v>16.999950131230705</v>
+      </c>
+      <c r="I2" s="22">
+        <f>H2-B2</f>
+        <v>-4.9868769295358106E-5</v>
+      </c>
+      <c r="J2">
         <v>10</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>1295</v>
       </c>
-      <c r="K2">
-        <f>J2/COS(RADIANS(I2))</f>
+      <c r="L2">
+        <f>K2/COS(RADIANS(J2))</f>
         <v>1314.9774623920398</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:12">
       <c r="A3">
         <f t="shared" si="0"/>
         <v>0.3490658503988659</v>
@@ -5244,23 +5527,31 @@
         <f t="shared" si="1"/>
         <v>0.36397023426620234</v>
       </c>
-      <c r="D3" s="13">
+      <c r="D3" s="12">
         <f t="shared" si="2"/>
         <v>478.61265504160701</v>
       </c>
       <c r="E3">
         <v>77</v>
       </c>
-      <c r="F3" s="13">
+      <c r="F3" s="12">
         <f t="shared" si="3"/>
         <v>401.61265504160701</v>
       </c>
-      <c r="G3" s="5">
+      <c r="G3" s="4">
         <f t="shared" ref="G3:G12" si="4">(F3-$D$2)/$D$2</f>
         <v>-1.0354991410686507E-3</v>
       </c>
-    </row>
-    <row r="4" spans="1:11">
+      <c r="H3" s="22">
+        <f>DEGREES(ATAN((E3+395.92)/1295))</f>
+        <v>20.061646955805756</v>
+      </c>
+      <c r="I3" s="22">
+        <f t="shared" ref="I3:I13" si="5">H3-B3</f>
+        <v>6.1646955805755965E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
       <c r="A4">
         <f t="shared" si="0"/>
         <v>0.39269908169872414</v>
@@ -5272,23 +5563,31 @@
         <f t="shared" si="1"/>
         <v>0.41421356237309503</v>
       </c>
-      <c r="D4" s="13">
+      <c r="D4" s="12">
         <f t="shared" si="2"/>
         <v>544.68149913773937</v>
       </c>
       <c r="E4">
         <v>141</v>
       </c>
-      <c r="F4" s="13">
+      <c r="F4" s="12">
         <f t="shared" si="3"/>
         <v>403.68149913773937</v>
       </c>
-      <c r="G4" s="5">
+      <c r="G4" s="4">
         <f t="shared" si="4"/>
         <v>4.1105085454513175E-3</v>
       </c>
-    </row>
-    <row r="5" spans="1:11">
+      <c r="H4" s="22">
+        <f t="shared" ref="H3:H13" si="6">DEGREES(ATAN((E4+395.92)/1295))</f>
+        <v>22.51938695477514</v>
+      </c>
+      <c r="I4" s="22">
+        <f t="shared" si="5"/>
+        <v>1.9386954775139742E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>0.43633231299858238</v>
@@ -5300,23 +5599,31 @@
         <f t="shared" si="1"/>
         <v>0.46630765815499858</v>
       </c>
-      <c r="D5" s="13">
+      <c r="D5" s="12">
         <f t="shared" si="2"/>
         <v>613.18406101463484</v>
       </c>
       <c r="E5">
         <v>209</v>
       </c>
-      <c r="F5" s="13">
+      <c r="F5" s="12">
         <f t="shared" si="3"/>
         <v>404.18406101463484</v>
       </c>
-      <c r="G5" s="5">
+      <c r="G5" s="4">
         <f t="shared" si="4"/>
         <v>5.3605724271574345E-3</v>
       </c>
-    </row>
-    <row r="6" spans="1:11">
+      <c r="H5" s="22">
+        <f t="shared" si="6"/>
+        <v>25.038204330616573</v>
+      </c>
+      <c r="I5" s="22">
+        <f t="shared" si="5"/>
+        <v>3.820433061657269E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>0.47996554429844063</v>
@@ -5328,23 +5635,31 @@
         <f t="shared" si="1"/>
         <v>0.52056705055174624</v>
       </c>
-      <c r="D6" s="13">
+      <c r="D6" s="12">
         <f t="shared" si="2"/>
         <v>684.53393913944399</v>
       </c>
       <c r="E6">
         <v>278</v>
       </c>
-      <c r="F6" s="13">
+      <c r="F6" s="12">
         <f t="shared" si="3"/>
         <v>406.53393913944399</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G6" s="4">
         <f t="shared" si="4"/>
         <v>1.1205619386113698E-2</v>
       </c>
-    </row>
-    <row r="7" spans="1:11">
+      <c r="H6" s="22">
+        <f t="shared" si="6"/>
+        <v>27.492538535873351</v>
+      </c>
+      <c r="I6" s="22">
+        <f t="shared" si="5"/>
+        <v>-7.4614641266492754E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>0.52359877559829882</v>
@@ -5356,23 +5671,31 @@
         <f t="shared" si="1"/>
         <v>0.57735026918962573</v>
       </c>
-      <c r="D7" s="13">
+      <c r="D7" s="12">
         <f t="shared" si="2"/>
         <v>759.20259189033516</v>
       </c>
       <c r="E7">
         <v>351</v>
       </c>
-      <c r="F7" s="13">
+      <c r="F7" s="12">
         <f t="shared" si="3"/>
         <v>408.20259189033516</v>
       </c>
-      <c r="G7" s="5">
+      <c r="G7" s="4">
         <f t="shared" si="4"/>
         <v>1.5356197913645871E-2</v>
       </c>
-    </row>
-    <row r="8" spans="1:11">
+      <c r="H7" s="22">
+        <f t="shared" si="6"/>
+        <v>29.975153121669841</v>
+      </c>
+      <c r="I7" s="22">
+        <f t="shared" si="5"/>
+        <v>-2.4846878330158972E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>0.56723200689815712</v>
@@ -5384,23 +5707,31 @@
         <f t="shared" si="1"/>
         <v>0.63707026080749318</v>
       </c>
-      <c r="D8" s="13">
+      <c r="D8" s="12">
         <f t="shared" si="2"/>
         <v>837.73303492207231</v>
       </c>
       <c r="E8">
         <v>427</v>
       </c>
-      <c r="F8" s="13">
+      <c r="F8" s="12">
         <f t="shared" si="3"/>
         <v>410.73303492207231</v>
       </c>
-      <c r="G8" s="5">
+      <c r="G8" s="4">
         <f t="shared" si="4"/>
         <v>2.1650378957042974E-2</v>
       </c>
-    </row>
-    <row r="9" spans="1:11">
+      <c r="H8" s="22">
+        <f t="shared" si="6"/>
+        <v>32.434303847596901</v>
+      </c>
+      <c r="I8" s="22">
+        <f t="shared" si="5"/>
+        <v>-6.5696152403099006E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>0.6108652381980153</v>
@@ -5412,23 +5743,31 @@
         <f t="shared" si="1"/>
         <v>0.70020753820970971</v>
       </c>
-      <c r="D9" s="13">
+      <c r="D9" s="12">
         <f t="shared" si="2"/>
         <v>920.75713174278133</v>
       </c>
       <c r="E9">
         <v>510</v>
       </c>
-      <c r="F9" s="13">
+      <c r="F9" s="12">
         <f t="shared" si="3"/>
         <v>410.75713174278133</v>
       </c>
-      <c r="G9" s="5">
+      <c r="G9" s="4">
         <f t="shared" si="4"/>
         <v>2.1710316979836053E-2</v>
       </c>
-    </row>
-    <row r="10" spans="1:11">
+      <c r="H9" s="22">
+        <f t="shared" si="6"/>
+        <v>34.974794138131706</v>
+      </c>
+      <c r="I9" s="22">
+        <f t="shared" si="5"/>
+        <v>-2.5205861868293766E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>0.6544984694978736</v>
@@ -5440,23 +5779,31 @@
         <f t="shared" si="1"/>
         <v>0.76732698797896037</v>
       </c>
-      <c r="D10" s="13">
+      <c r="D10" s="12">
         <f t="shared" si="2"/>
         <v>1009.0176954775005</v>
       </c>
       <c r="E10">
         <v>593</v>
       </c>
-      <c r="F10" s="13">
+      <c r="F10" s="12">
         <f t="shared" si="3"/>
         <v>416.01769547750052</v>
       </c>
-      <c r="G10" s="5">
+      <c r="G10" s="4">
         <f t="shared" si="4"/>
         <v>3.4795353916597743E-2</v>
       </c>
-    </row>
-    <row r="11" spans="1:11">
+      <c r="H10" s="22">
+        <f t="shared" si="6"/>
+        <v>37.36697428663765</v>
+      </c>
+      <c r="I10" s="22">
+        <f t="shared" si="5"/>
+        <v>-0.13302571336235047</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>0.69813170079773179</v>
@@ -5468,23 +5815,31 @@
         <f t="shared" si="1"/>
         <v>0.83909963117727993</v>
       </c>
-      <c r="D11" s="13">
+      <c r="D11" s="12">
         <f t="shared" si="2"/>
         <v>1103.3971036995961</v>
       </c>
       <c r="E11">
         <v>684</v>
       </c>
-      <c r="F11" s="13">
+      <c r="F11" s="12">
         <f t="shared" si="3"/>
         <v>419.39710369959607</v>
       </c>
-      <c r="G11" s="5">
+      <c r="G11" s="4">
         <f t="shared" si="4"/>
         <v>4.3201236563484222E-2</v>
       </c>
-    </row>
-    <row r="12" spans="1:11">
+      <c r="H11" s="22">
+        <f>DEGREES(ATAN((E11+395.92)/1295))</f>
+        <v>39.825235843907642</v>
+      </c>
+      <c r="I11" s="22">
+        <f t="shared" si="5"/>
+        <v>-0.17476415609235829</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>0.73303828583761843</v>
@@ -5496,148 +5851,160 @@
         <f t="shared" si="1"/>
         <v>0.90040404429783993</v>
       </c>
-      <c r="D12" s="13">
+      <c r="D12" s="12">
         <f t="shared" si="2"/>
         <v>1184.0110252983034</v>
       </c>
       <c r="E12">
         <v>760</v>
       </c>
-      <c r="F12" s="13">
+      <c r="F12" s="12">
         <f t="shared" si="3"/>
         <v>424.01102529830337</v>
       </c>
-      <c r="G12" s="5">
+      <c r="G12" s="4">
         <f t="shared" si="4"/>
         <v>5.4677826827746107E-2</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" ht="15" customHeight="1">
-      <c r="B14" s="13">
+      <c r="H12" s="22">
+        <f t="shared" si="6"/>
+        <v>41.752174638684821</v>
+      </c>
+      <c r="I12" s="22">
+        <f t="shared" si="5"/>
+        <v>-0.24782536131517929</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="15" customHeight="1">
+      <c r="H13" s="22"/>
+      <c r="I13" s="22"/>
+    </row>
+    <row r="14" spans="1:12" ht="15" customHeight="1">
+      <c r="B14" s="12">
         <f>D2-$D$2</f>
         <v>0</v>
       </c>
-      <c r="C14" s="13">
+      <c r="C14" s="12">
         <f>B14-E2</f>
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="15" customHeight="1">
-      <c r="B15" s="13">
-        <f t="shared" ref="B15:B24" si="5">D3-$D$2</f>
+    <row r="15" spans="1:12" ht="15" customHeight="1">
+      <c r="B15" s="12">
+        <f t="shared" ref="B15:B24" si="7">D3-$D$2</f>
         <v>76.583699361708739</v>
       </c>
-      <c r="C15" s="13">
-        <f t="shared" ref="C15:C24" si="6">B15-E3</f>
+      <c r="C15" s="12">
+        <f t="shared" ref="C15:C24" si="8">B15-E3</f>
         <v>-0.41630063829126129</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15" customHeight="1">
-      <c r="B16" s="13">
-        <f t="shared" si="5"/>
+    <row r="16" spans="1:12" ht="15" customHeight="1">
+      <c r="B16" s="12">
+        <f t="shared" si="7"/>
         <v>142.65254345784109</v>
       </c>
-      <c r="C16" s="13">
-        <f t="shared" si="6"/>
+      <c r="C16" s="12">
+        <f t="shared" si="8"/>
         <v>1.6525434578410909</v>
       </c>
     </row>
     <row r="17" spans="2:6" ht="15" customHeight="1">
-      <c r="B17" s="13">
-        <f t="shared" si="5"/>
+      <c r="B17" s="12">
+        <f t="shared" si="7"/>
         <v>211.15510533473656</v>
       </c>
-      <c r="C17" s="13">
-        <f t="shared" si="6"/>
+      <c r="C17" s="12">
+        <f t="shared" si="8"/>
         <v>2.155105334736561</v>
       </c>
     </row>
     <row r="18" spans="2:6" ht="15" customHeight="1">
-      <c r="B18" s="13">
-        <f t="shared" si="5"/>
+      <c r="B18" s="12">
+        <f t="shared" si="7"/>
         <v>282.50498345954571</v>
       </c>
-      <c r="C18" s="13">
-        <f t="shared" si="6"/>
+      <c r="C18" s="12">
+        <f t="shared" si="8"/>
         <v>4.5049834595457128</v>
       </c>
     </row>
     <row r="19" spans="2:6" ht="15" customHeight="1">
-      <c r="B19" s="13">
-        <f t="shared" si="5"/>
+      <c r="B19" s="12">
+        <f t="shared" si="7"/>
         <v>357.17363621043688</v>
       </c>
-      <c r="C19" s="13">
-        <f t="shared" si="6"/>
+      <c r="C19" s="12">
+        <f t="shared" si="8"/>
         <v>6.1736362104368823</v>
       </c>
     </row>
     <row r="20" spans="2:6" ht="15" customHeight="1">
-      <c r="B20" s="13">
-        <f t="shared" si="5"/>
+      <c r="B20" s="12">
+        <f t="shared" si="7"/>
         <v>435.70407924217403</v>
       </c>
-      <c r="C20" s="13">
-        <f t="shared" si="6"/>
+      <c r="C20" s="12">
+        <f t="shared" si="8"/>
         <v>8.7040792421740321</v>
       </c>
     </row>
     <row r="21" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B21" s="13">
-        <f t="shared" si="5"/>
+      <c r="B21" s="12">
+        <f t="shared" si="7"/>
         <v>518.72817606288299</v>
       </c>
-      <c r="C21" s="13">
-        <f t="shared" si="6"/>
+      <c r="C21" s="12">
+        <f t="shared" si="8"/>
         <v>8.7281760628829943</v>
       </c>
     </row>
     <row r="22" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B22" s="13">
-        <f t="shared" si="5"/>
+      <c r="B22" s="12">
+        <f t="shared" si="7"/>
         <v>606.98873979760219</v>
       </c>
-      <c r="C22" s="13">
-        <f t="shared" si="6"/>
+      <c r="C22" s="12">
+        <f t="shared" si="8"/>
         <v>13.988739797602193</v>
       </c>
     </row>
     <row r="23" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B23" s="13">
-        <f t="shared" si="5"/>
+      <c r="B23" s="12">
+        <f t="shared" si="7"/>
         <v>701.36814801969786</v>
       </c>
-      <c r="C23" s="13">
-        <f t="shared" si="6"/>
+      <c r="C23" s="12">
+        <f t="shared" si="8"/>
         <v>17.368148019697855</v>
       </c>
     </row>
     <row r="24" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B24" s="13">
-        <f t="shared" si="5"/>
+      <c r="B24" s="12">
+        <f t="shared" si="7"/>
         <v>781.98206961840515</v>
       </c>
-      <c r="C24" s="13">
-        <f t="shared" si="6"/>
+      <c r="C24" s="12">
+        <f t="shared" si="8"/>
         <v>21.982069618405149</v>
       </c>
     </row>
     <row r="25" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B25" s="13"/>
+      <c r="B25" s="12"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
     </row>
     <row r="26" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B26" s="13"/>
+      <c r="B26" s="12"/>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
     </row>
     <row r="27" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B27" s="13"/>
+      <c r="B27" s="12"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
@@ -6670,7 +7037,7 @@
   <dimension ref="A1:K1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="I40" sqref="I40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>